<commit_message>
added api document and updated product backlog
</commit_message>
<xml_diff>
--- a/SSW695/product backlog.xlsx
+++ b/SSW695/product backlog.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
   <si>
     <t>User Story</t>
   </si>
@@ -95,10 +95,10 @@
     <t>Pranay, Sonali</t>
   </si>
   <si>
-    <t>Create Api for post issue and get issue feed</t>
-  </si>
-  <si>
-    <t>Create Api for forgot password and get issue history for user</t>
+    <t>Create Api for post issue and get issue feed/history</t>
+  </si>
+  <si>
+    <t>Create Api for forgot and reset password</t>
   </si>
   <si>
     <t>Create Api for update settings</t>
@@ -107,21 +107,36 @@
     <t>Create Api for add maintenance personnel</t>
   </si>
   <si>
-    <t>Create Api to get list of users, maintenance personnel</t>
-  </si>
-  <si>
-    <t>Create Api to information about particular issue, user and maintenance person</t>
+    <t>This api is merged with registration api.</t>
+  </si>
+  <si>
+    <t>Create Api to get list of users</t>
+  </si>
+  <si>
+    <t>Create Api to information about particular issue, user</t>
   </si>
   <si>
     <t>Create Api to update issue, user or maintenance person</t>
   </si>
   <si>
+    <t>This api is merged with update issue api</t>
+  </si>
+  <si>
     <t>Create Api to assign issue to a maintenance person</t>
   </si>
   <si>
     <t>This api can be included in update issue api.</t>
   </si>
   <si>
+    <t>Create api to add category, priorities from CMS</t>
+  </si>
+  <si>
+    <t>Create api to update categories, priorities from CMS</t>
+  </si>
+  <si>
+    <t>Create api to delete categories, priorities from CMS</t>
+  </si>
+  <si>
     <t>Create login, home page in CMS</t>
   </si>
   <si>
@@ -144,6 +159,9 @@
   </si>
   <si>
     <t>Create user list page, maintenance personnel list page</t>
+  </si>
+  <si>
+    <t>Create page to add, update or delete categories and priorities in CMS</t>
   </si>
   <si>
     <t>Fill database tables categories and priorities</t>
@@ -1378,7 +1396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1619,7 +1637,7 @@
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" ht="15" customHeight="1">
+    <row r="16" ht="31" customHeight="1">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1669,14 +1687,16 @@
         <v>26</v>
       </c>
       <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="E19" t="s" s="7">
+        <v>31</v>
+      </c>
     </row>
     <row r="20" ht="29" customHeight="1">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s" s="4">
         <v>26</v>
@@ -1689,7 +1709,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s" s="7">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s" s="7">
         <v>26</v>
@@ -1702,60 +1722,58 @@
         <v>21</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s" s="4">
         <v>26</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="E22" t="s" s="4">
+        <v>35</v>
+      </c>
     </row>
     <row r="23" ht="29" customHeight="1">
       <c r="A23" s="6">
         <v>22</v>
       </c>
       <c r="B23" t="s" s="7">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s" s="7">
         <v>26</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" t="s" s="7">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" ht="43" customHeight="1">
-      <c r="A24" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" ht="29" customHeight="1">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" t="s" s="4">
-        <v>36</v>
-      </c>
-      <c r="C24" t="s" s="4">
-        <v>37</v>
-      </c>
-      <c r="D24" t="s" s="4">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s" s="4">
+      <c r="B24" t="s" s="7">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" ht="15" customHeight="1">
-      <c r="A25" s="6">
+      <c r="C24" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" ht="43" customHeight="1">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" t="s" s="7">
+      <c r="B25" t="s" s="4">
         <v>39</v>
       </c>
-      <c r="C25" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" ht="29" customHeight="1">
+      <c r="C25" t="s" s="4">
+        <v>26</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" ht="43" customHeight="1">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1763,81 +1781,109 @@
         <v>40</v>
       </c>
       <c r="C26" t="s" s="4">
-        <v>37</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" ht="55.2" customHeight="1">
-      <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" t="s" s="7">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" ht="43" customHeight="1">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s" s="4">
         <v>41</v>
       </c>
-      <c r="C27" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" t="s" s="7">
+      <c r="C27" t="s" s="4">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" ht="29" customHeight="1">
-      <c r="A28" s="3">
+      <c r="D27" t="s" s="4">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s" s="4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" ht="15" customHeight="1">
+      <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="B28" t="s" s="4">
-        <v>43</v>
-      </c>
-      <c r="C28" t="s" s="4">
-        <v>37</v>
-      </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" ht="15" customHeight="1">
-      <c r="A29" s="6">
+      <c r="B28" t="s" s="7">
+        <v>44</v>
+      </c>
+      <c r="C28" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" ht="29" customHeight="1">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C29" t="s" s="7">
+      <c r="B29" t="s" s="4">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s" s="4">
+        <v>42</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" ht="55.2" customHeight="1">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" t="s" s="7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" ht="29" customHeight="1">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s" s="4">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s" s="4">
+        <v>42</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" ht="31" customHeight="1">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" ht="15" customHeight="1">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s" s="7">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s" s="7">
         <v>18</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" ht="15" customHeight="1">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" ht="15" customHeight="1">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" ht="15" customHeight="1">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" ht="15" customHeight="1">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" ht="15.6" customHeight="1">
+    <row r="34" ht="15" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1865,7 +1911,7 @@
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" ht="15" customHeight="1">
+    <row r="38" ht="15.6" customHeight="1">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1935,49 +1981,49 @@
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
     </row>
-    <row r="48" ht="31.2" customHeight="1">
+    <row r="48" ht="15" customHeight="1">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" ht="31.2" customHeight="1">
+    <row r="49" ht="15" customHeight="1">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
     </row>
-    <row r="50" ht="31.2" customHeight="1">
+    <row r="50" ht="15" customHeight="1">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" ht="18.6" customHeight="1">
+    <row r="51" ht="15" customHeight="1">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
     </row>
-    <row r="52" ht="18.6" customHeight="1">
+    <row r="52" ht="31.2" customHeight="1">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
-    <row r="53" ht="18.6" customHeight="1">
+    <row r="53" ht="31.2" customHeight="1">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
     </row>
-    <row r="54" ht="18.6" customHeight="1">
+    <row r="54" ht="31.2" customHeight="1">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -2067,6 +2113,34 @@
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
+    </row>
+    <row r="67" ht="18.6" customHeight="1">
+      <c r="A67" s="8"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+    </row>
+    <row r="68" ht="18.6" customHeight="1">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+    </row>
+    <row r="69" ht="18.6" customHeight="1">
+      <c r="A69" s="8"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+    </row>
+    <row r="70" ht="18.6" customHeight="1">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2124,7 +2198,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s" s="12">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" ht="18.6" customHeight="1">
@@ -2327,10 +2401,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s" s="12">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s" s="12">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s" s="12">
         <v>7</v>

</xml_diff>

<commit_message>
Updated product backlog for Oct30 - Nov3.
</commit_message>
<xml_diff>
--- a/SSW695/product backlog.xlsx
+++ b/SSW695/product backlog.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stevens data\3rd SEM\SSW_Capstone\SSW695_Team7\SSW695\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="product backlog" sheetId="1" r:id="rId4"/>
-    <sheet name="Oct23 - Oct27" sheetId="2" r:id="rId5"/>
+    <sheet name="product backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Oct23 - Oct27" sheetId="2" r:id="rId2"/>
+    <sheet name="Oct30 - Nov3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="52">
   <si>
     <t>User Story</t>
   </si>
@@ -173,28 +182,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -257,61 +253,62 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -321,27 +318,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffcacaca"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffe6e6e6"/>
-      <rgbColor rgb="ffe0e0e0"/>
-      <rgbColor rgb="fff0f0f0"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFCACACA"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFE6E6E6"/>
+      <rgbColor rgb="FFE0E0E0"/>
+      <rgbColor rgb="FFF0F0F0"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -543,7 +598,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -562,7 +617,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -592,7 +647,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -618,7 +673,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -644,7 +699,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -670,7 +725,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -696,7 +751,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -722,7 +777,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -748,7 +803,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -774,7 +829,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -800,7 +855,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -813,9 +868,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -832,7 +893,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -851,7 +912,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -877,7 +938,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -903,7 +964,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -929,7 +990,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -955,7 +1016,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -981,7 +1042,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1007,7 +1068,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1033,7 +1094,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1059,7 +1120,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1085,7 +1146,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1098,9 +1159,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1114,7 +1181,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1133,7 +1200,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1163,7 +1230,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1189,7 +1256,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1215,7 +1282,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1241,7 +1308,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1267,7 +1334,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1293,7 +1360,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1319,7 +1386,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1345,7 +1412,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1371,7 +1438,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1384,758 +1451,767 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV70"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:E22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6667" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="44" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="69.6719" style="1" customWidth="1"/>
-    <col min="6" max="256" width="10.6719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="69.6640625" style="1" customWidth="1"/>
+    <col min="6" max="256" width="10.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="C3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="D3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" ht="29" customHeight="1">
+    <row r="4" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="4">
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="7">
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s" s="7">
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s" s="7">
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s" s="4">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" ht="29" customHeight="1">
+    <row r="7" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="7">
+      <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s" s="7">
+      <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s" s="7">
+      <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" ht="29" customHeight="1">
+    <row r="8" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="4">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s" s="4">
+      <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s" s="4">
+      <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" ht="29" customHeight="1">
+    <row r="9" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="7">
+      <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s" s="7">
+      <c r="C9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s" s="7">
+      <c r="D9" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="4">
+      <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s" s="4">
+      <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s" s="4">
+      <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="7">
+      <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s" s="7">
+      <c r="C11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D11" t="s" s="7">
+      <c r="D11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" t="s" s="4">
+      <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s" s="4">
+      <c r="C12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s" s="4">
+      <c r="D12" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" t="s" s="7">
+      <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s" s="7">
+      <c r="C13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s" s="7">
+      <c r="D13" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" t="s" s="4">
+      <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s" s="4">
+      <c r="C14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D14" t="s" s="4">
+      <c r="D14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" t="s" s="7">
+      <c r="B15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s" s="7">
+      <c r="C15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D15" t="s" s="7">
+      <c r="D15" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" ht="31" customHeight="1">
+    <row r="16" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" t="s" s="4">
+      <c r="B16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C16" t="s" s="4">
+      <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" ht="29" customHeight="1">
+    <row r="17" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" t="s" s="7">
+      <c r="B17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C17" t="s" s="7">
+      <c r="C17" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" t="s" s="4">
+      <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C18" t="s" s="4">
+      <c r="C18" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" ht="15" customHeight="1">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" t="s" s="7">
+      <c r="B19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C19" t="s" s="7">
+      <c r="C19" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="8"/>
-      <c r="E19" t="s" s="7">
+      <c r="E19" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" ht="29" customHeight="1">
+    <row r="20" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" t="s" s="4">
+      <c r="B20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C20" t="s" s="4">
+      <c r="C20" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" ht="29" customHeight="1">
+    <row r="21" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>20</v>
       </c>
-      <c r="B21" t="s" s="7">
+      <c r="B21" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C21" t="s" s="7">
+      <c r="C21" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" ht="29" customHeight="1">
+    <row r="22" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" t="s" s="4">
+      <c r="B22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C22" t="s" s="4">
+      <c r="C22" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" t="s" s="4">
+      <c r="E22" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" ht="29" customHeight="1">
+    <row r="23" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" t="s" s="7">
+      <c r="B23" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C23" t="s" s="7">
+      <c r="C23" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="8"/>
-      <c r="E23" t="s" s="7">
+      <c r="E23" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" ht="29" customHeight="1">
+    <row r="24" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" t="s" s="7">
+      <c r="B24" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C24" t="s" s="7">
+      <c r="C24" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" ht="43" customHeight="1">
+    <row r="25" spans="1:5" ht="43" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" t="s" s="4">
+      <c r="B25" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C25" t="s" s="4">
+      <c r="C25" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" ht="43" customHeight="1">
+    <row r="26" spans="1:5" ht="43" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" t="s" s="4">
+      <c r="B26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C26" t="s" s="4">
+      <c r="C26" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" ht="43" customHeight="1">
+    <row r="27" spans="1:5" ht="43" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" t="s" s="4">
+      <c r="B27" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C27" t="s" s="4">
+      <c r="C27" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D27" t="s" s="4">
-        <v>7</v>
-      </c>
-      <c r="E27" t="s" s="4">
+      <c r="D27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" ht="15" customHeight="1">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="B28" t="s" s="7">
+      <c r="B28" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C28" t="s" s="7">
+      <c r="C28" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" ht="29" customHeight="1">
+    <row r="29" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" t="s" s="4">
+      <c r="B29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C29" t="s" s="4">
+      <c r="C29" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" ht="55.2" customHeight="1">
+    <row r="30" spans="1:5" ht="55.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>29</v>
       </c>
-      <c r="B30" t="s" s="7">
+      <c r="B30" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C30" t="s" s="7">
+      <c r="C30" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D30" s="8"/>
-      <c r="E30" t="s" s="7">
+      <c r="E30" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" ht="29" customHeight="1">
+    <row r="31" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
-      <c r="B31" t="s" s="4">
+      <c r="B31" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C31" t="s" s="4">
+      <c r="C31" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" ht="31" customHeight="1">
+    <row r="32" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>31</v>
       </c>
-      <c r="B32" t="s" s="7">
+      <c r="B32" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C32" t="s" s="7">
+      <c r="C32" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" ht="15" customHeight="1">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>32</v>
       </c>
-      <c r="B33" t="s" s="7">
+      <c r="B33" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C33" t="s" s="7">
+      <c r="C33" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" ht="15" customHeight="1">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" ht="15" customHeight="1">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" ht="15" customHeight="1">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" ht="15" customHeight="1">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" ht="15.6" customHeight="1">
+    <row r="38" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" ht="15" customHeight="1">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" ht="15" customHeight="1">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" ht="15" customHeight="1">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" ht="15" customHeight="1">
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" ht="15" customHeight="1">
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
     </row>
-    <row r="44" ht="15" customHeight="1">
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" ht="15" customHeight="1">
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" ht="15" customHeight="1">
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
     </row>
-    <row r="47" ht="15" customHeight="1">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
     </row>
-    <row r="48" ht="15" customHeight="1">
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" ht="15" customHeight="1">
+    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
     </row>
-    <row r="50" ht="15" customHeight="1">
+    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" ht="15" customHeight="1">
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
     </row>
-    <row r="52" ht="31.2" customHeight="1">
+    <row r="52" spans="1:5" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
-    <row r="53" ht="31.2" customHeight="1">
+    <row r="53" spans="1:5" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
     </row>
-    <row r="54" ht="31.2" customHeight="1">
+    <row r="54" spans="1:5" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" ht="18.6" customHeight="1">
+    <row r="55" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
     </row>
-    <row r="56" ht="18.6" customHeight="1">
+    <row r="56" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
     </row>
-    <row r="57" ht="18.6" customHeight="1">
+    <row r="57" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" ht="18.6" customHeight="1">
+    <row r="58" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" ht="18.6" customHeight="1">
+    <row r="59" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
     </row>
-    <row r="60" ht="18.6" customHeight="1">
+    <row r="60" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
     </row>
-    <row r="61" ht="18.6" customHeight="1">
+    <row r="61" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
     </row>
-    <row r="62" ht="18.6" customHeight="1">
+    <row r="62" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
     </row>
-    <row r="63" ht="18.6" customHeight="1">
+    <row r="63" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
     </row>
-    <row r="64" ht="18.6" customHeight="1">
+    <row r="64" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
     </row>
-    <row r="65" ht="18.6" customHeight="1">
+    <row r="65" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
     </row>
-    <row r="66" ht="18.6" customHeight="1">
+    <row r="66" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
     </row>
-    <row r="67" ht="18.6" customHeight="1">
+    <row r="67" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
     </row>
-    <row r="68" ht="18.6" customHeight="1">
+    <row r="68" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
     </row>
-    <row r="69" ht="18.6" customHeight="1">
+    <row r="69" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
       <c r="E69" s="8"/>
     </row>
-    <row r="70" ht="18.6" customHeight="1">
+    <row r="70" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -2144,7 +2220,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2152,350 +2228,352 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV29"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.6719" style="9" customWidth="1"/>
-    <col min="2" max="2" width="45.8516" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.3516" style="9" customWidth="1"/>
-    <col min="4" max="4" width="12.6719" style="9" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="9" customWidth="1"/>
     <col min="5" max="5" width="38.5" style="9" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="9" customWidth="1"/>
+    <col min="6" max="256" width="8.83203125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1">
-      <c r="A1" t="s" s="10">
+    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="10">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="10">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="10">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="10">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="40.5" customHeight="1">
+    <row r="2" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="12">
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="12">
+      <c r="C2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s" s="12">
+      <c r="D2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" ht="18.6" customHeight="1">
+    <row r="3" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="10">
+      <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="10">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s" s="10">
-        <v>7</v>
-      </c>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" ht="29" customHeight="1">
+      <c r="D3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="12">
+      <c r="B4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s" s="12">
+      <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="E4" s="15"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
+      <c r="D4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="10">
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s" s="10">
+      <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s" s="10">
-        <v>7</v>
-      </c>
-      <c r="E5" s="14"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
+      <c r="D5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="12">
+      <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s" s="12">
+      <c r="C6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" ht="29" customHeight="1">
+      <c r="D6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="10">
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s" s="10">
+      <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s" s="10">
-        <v>7</v>
-      </c>
-      <c r="E7" s="14"/>
-    </row>
-    <row r="8" ht="18.6" customHeight="1">
+      <c r="D7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="12">
+      <c r="B8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s" s="12">
+      <c r="C8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" ht="29" customHeight="1">
+      <c r="D8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="10">
+      <c r="B9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s" s="10">
+      <c r="C9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s" s="10">
-        <v>7</v>
-      </c>
-      <c r="E9" s="14"/>
-    </row>
-    <row r="10" ht="18.6" customHeight="1">
+      <c r="D9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="12">
+      <c r="B10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s" s="12">
+      <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="E10" s="15"/>
-    </row>
-    <row r="11" ht="18.6" customHeight="1">
+      <c r="D10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="10">
+      <c r="B11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s" s="10">
+      <c r="C11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D11" t="s" s="10">
+      <c r="D11" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="14"/>
     </row>
-    <row r="12" ht="18.6" customHeight="1">
+    <row r="12" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" t="s" s="12">
+      <c r="B12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s" s="12">
+      <c r="C12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s" s="12">
+      <c r="D12" s="12" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" ht="55.8" customHeight="1">
+    <row r="13" spans="1:5" ht="55.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13">
         <v>12</v>
       </c>
-      <c r="B13" t="s" s="10">
+      <c r="B13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s" s="10">
+      <c r="C13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s" s="10">
+      <c r="D13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" ht="37.2" customHeight="1">
+    <row r="14" spans="1:5" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>13</v>
       </c>
-      <c r="B14" t="s" s="12">
+      <c r="B14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s" s="12">
+      <c r="C14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D14" t="s" s="12">
+      <c r="D14" s="12" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" ht="37.2" customHeight="1">
+    <row r="15" spans="1:5" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13">
         <v>14</v>
       </c>
-      <c r="B15" t="s" s="10">
+      <c r="B15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s" s="10">
+      <c r="C15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D15" t="s" s="10">
-        <v>7</v>
+      <c r="D15" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" ht="18.6" customHeight="1">
+    <row r="16" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11">
         <v>15</v>
       </c>
-      <c r="B16" t="s" s="12">
+      <c r="B16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C16" t="s" s="12">
+      <c r="C16" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D16" t="s" s="12">
+      <c r="D16" s="12" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="15"/>
     </row>
-    <row r="17" ht="18.6" customHeight="1">
+    <row r="17" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="18" ht="37.2" customHeight="1">
+    <row r="18" spans="1:5" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" ht="37.2" customHeight="1">
+    <row r="19" spans="1:5" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
     </row>
-    <row r="20" ht="37.2" customHeight="1">
+    <row r="20" spans="1:5" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" ht="18.6" customHeight="1">
+    <row r="21" spans="1:5" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
     </row>
-    <row r="22" ht="15" customHeight="1">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" ht="15" customHeight="1">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
     </row>
-    <row r="24" ht="15" customHeight="1">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" ht="15" customHeight="1">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
     </row>
-    <row r="26" ht="15" customHeight="1">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
     </row>
-    <row r="27" ht="15" customHeight="1">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
     </row>
-    <row r="28" ht="15" customHeight="1">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="15"/>
       <c r="B28" s="12"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
     </row>
-    <row r="29" ht="15" customHeight="1">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="14"/>
       <c r="B29" s="10"/>
       <c r="C29" s="14"/>
@@ -2507,9 +2585,110 @@
     <mergeCell ref="E2:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>18</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>21</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>23</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Priority, Category API.
</commit_message>
<xml_diff>
--- a/SSW695/product backlog.xlsx
+++ b/SSW695/product backlog.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stevens data\3rd SEM\SSW_Capstone\SSW695_Team7\SSW695\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="product backlog" sheetId="1" r:id="rId4"/>
-    <sheet name="Oct23 - Oct29" sheetId="2" r:id="rId5"/>
-    <sheet name="Oct30 - Nov5" sheetId="3" r:id="rId6"/>
+    <sheet name="product backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Oct23 - Oct29" sheetId="2" r:id="rId2"/>
+    <sheet name="Oct30 - Nov5" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="101">
   <si>
     <t>User Story</t>
   </si>
@@ -321,36 +329,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="7">
@@ -540,96 +530,75 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="32">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -640,28 +609,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffcacaca"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffe6e6e6"/>
-      <rgbColor rgb="ffe0e0e0"/>
-      <rgbColor rgb="fff0f0f0"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFCACACA"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFE6E6E6"/>
+      <rgbColor rgb="FFE0E0E0"/>
+      <rgbColor rgb="FFF0F0F0"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -863,7 +889,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -882,7 +908,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -912,7 +938,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -938,7 +964,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -964,7 +990,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -990,7 +1016,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1016,7 +1042,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1042,7 +1068,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1068,7 +1094,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1094,7 +1120,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1120,7 +1146,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1133,9 +1159,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1152,7 +1184,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1171,7 +1203,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1197,7 +1229,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1223,7 +1255,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1249,7 +1281,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1275,7 +1307,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1301,7 +1333,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1327,7 +1359,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1353,7 +1385,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1379,7 +1411,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1405,7 +1437,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1418,9 +1450,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1434,7 +1472,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1453,7 +1491,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1483,7 +1521,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1509,7 +1547,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1535,7 +1573,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1561,7 +1599,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1587,7 +1625,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1613,7 +1651,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1639,7 +1677,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1665,7 +1703,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1691,7 +1729,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1704,295 +1742,55 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IU81"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6667" defaultRowHeight="14" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="44" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="69.6719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6719" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6719" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6719" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6719" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6719" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6719" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6719" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6719" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6719" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.6719" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.6719" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6719" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.6719" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10.6719" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.6719" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.6719" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.6719" style="1" customWidth="1"/>
-    <col min="23" max="23" width="10.6719" style="1" customWidth="1"/>
-    <col min="24" max="24" width="10.6719" style="1" customWidth="1"/>
-    <col min="25" max="25" width="10.6719" style="1" customWidth="1"/>
-    <col min="26" max="26" width="10.6719" style="1" customWidth="1"/>
-    <col min="27" max="27" width="10.6719" style="1" customWidth="1"/>
-    <col min="28" max="28" width="10.6719" style="1" customWidth="1"/>
-    <col min="29" max="29" width="10.6719" style="1" customWidth="1"/>
-    <col min="30" max="30" width="10.6719" style="1" customWidth="1"/>
-    <col min="31" max="31" width="10.6719" style="1" customWidth="1"/>
-    <col min="32" max="32" width="10.6719" style="1" customWidth="1"/>
-    <col min="33" max="33" width="10.6719" style="1" customWidth="1"/>
-    <col min="34" max="34" width="10.6719" style="1" customWidth="1"/>
-    <col min="35" max="35" width="10.6719" style="1" customWidth="1"/>
-    <col min="36" max="36" width="10.6719" style="1" customWidth="1"/>
-    <col min="37" max="37" width="10.6719" style="1" customWidth="1"/>
-    <col min="38" max="38" width="10.6719" style="1" customWidth="1"/>
-    <col min="39" max="39" width="10.6719" style="1" customWidth="1"/>
-    <col min="40" max="40" width="10.6719" style="1" customWidth="1"/>
-    <col min="41" max="41" width="10.6719" style="1" customWidth="1"/>
-    <col min="42" max="42" width="10.6719" style="1" customWidth="1"/>
-    <col min="43" max="43" width="10.6719" style="1" customWidth="1"/>
-    <col min="44" max="44" width="10.6719" style="1" customWidth="1"/>
-    <col min="45" max="45" width="10.6719" style="1" customWidth="1"/>
-    <col min="46" max="46" width="10.6719" style="1" customWidth="1"/>
-    <col min="47" max="47" width="10.6719" style="1" customWidth="1"/>
-    <col min="48" max="48" width="10.6719" style="1" customWidth="1"/>
-    <col min="49" max="49" width="10.6719" style="1" customWidth="1"/>
-    <col min="50" max="50" width="10.6719" style="1" customWidth="1"/>
-    <col min="51" max="51" width="10.6719" style="1" customWidth="1"/>
-    <col min="52" max="52" width="10.6719" style="1" customWidth="1"/>
-    <col min="53" max="53" width="10.6719" style="1" customWidth="1"/>
-    <col min="54" max="54" width="10.6719" style="1" customWidth="1"/>
-    <col min="55" max="55" width="10.6719" style="1" customWidth="1"/>
-    <col min="56" max="56" width="10.6719" style="1" customWidth="1"/>
-    <col min="57" max="57" width="10.6719" style="1" customWidth="1"/>
-    <col min="58" max="58" width="10.6719" style="1" customWidth="1"/>
-    <col min="59" max="59" width="10.6719" style="1" customWidth="1"/>
-    <col min="60" max="60" width="10.6719" style="1" customWidth="1"/>
-    <col min="61" max="61" width="10.6719" style="1" customWidth="1"/>
-    <col min="62" max="62" width="10.6719" style="1" customWidth="1"/>
-    <col min="63" max="63" width="10.6719" style="1" customWidth="1"/>
-    <col min="64" max="64" width="10.6719" style="1" customWidth="1"/>
-    <col min="65" max="65" width="10.6719" style="1" customWidth="1"/>
-    <col min="66" max="66" width="10.6719" style="1" customWidth="1"/>
-    <col min="67" max="67" width="10.6719" style="1" customWidth="1"/>
-    <col min="68" max="68" width="10.6719" style="1" customWidth="1"/>
-    <col min="69" max="69" width="10.6719" style="1" customWidth="1"/>
-    <col min="70" max="70" width="10.6719" style="1" customWidth="1"/>
-    <col min="71" max="71" width="10.6719" style="1" customWidth="1"/>
-    <col min="72" max="72" width="10.6719" style="1" customWidth="1"/>
-    <col min="73" max="73" width="10.6719" style="1" customWidth="1"/>
-    <col min="74" max="74" width="10.6719" style="1" customWidth="1"/>
-    <col min="75" max="75" width="10.6719" style="1" customWidth="1"/>
-    <col min="76" max="76" width="10.6719" style="1" customWidth="1"/>
-    <col min="77" max="77" width="10.6719" style="1" customWidth="1"/>
-    <col min="78" max="78" width="10.6719" style="1" customWidth="1"/>
-    <col min="79" max="79" width="10.6719" style="1" customWidth="1"/>
-    <col min="80" max="80" width="10.6719" style="1" customWidth="1"/>
-    <col min="81" max="81" width="10.6719" style="1" customWidth="1"/>
-    <col min="82" max="82" width="10.6719" style="1" customWidth="1"/>
-    <col min="83" max="83" width="10.6719" style="1" customWidth="1"/>
-    <col min="84" max="84" width="10.6719" style="1" customWidth="1"/>
-    <col min="85" max="85" width="10.6719" style="1" customWidth="1"/>
-    <col min="86" max="86" width="10.6719" style="1" customWidth="1"/>
-    <col min="87" max="87" width="10.6719" style="1" customWidth="1"/>
-    <col min="88" max="88" width="10.6719" style="1" customWidth="1"/>
-    <col min="89" max="89" width="10.6719" style="1" customWidth="1"/>
-    <col min="90" max="90" width="10.6719" style="1" customWidth="1"/>
-    <col min="91" max="91" width="10.6719" style="1" customWidth="1"/>
-    <col min="92" max="92" width="10.6719" style="1" customWidth="1"/>
-    <col min="93" max="93" width="10.6719" style="1" customWidth="1"/>
-    <col min="94" max="94" width="10.6719" style="1" customWidth="1"/>
-    <col min="95" max="95" width="10.6719" style="1" customWidth="1"/>
-    <col min="96" max="96" width="10.6719" style="1" customWidth="1"/>
-    <col min="97" max="97" width="10.6719" style="1" customWidth="1"/>
-    <col min="98" max="98" width="10.6719" style="1" customWidth="1"/>
-    <col min="99" max="99" width="10.6719" style="1" customWidth="1"/>
-    <col min="100" max="100" width="10.6719" style="1" customWidth="1"/>
-    <col min="101" max="101" width="10.6719" style="1" customWidth="1"/>
-    <col min="102" max="102" width="10.6719" style="1" customWidth="1"/>
-    <col min="103" max="103" width="10.6719" style="1" customWidth="1"/>
-    <col min="104" max="104" width="10.6719" style="1" customWidth="1"/>
-    <col min="105" max="105" width="10.6719" style="1" customWidth="1"/>
-    <col min="106" max="106" width="10.6719" style="1" customWidth="1"/>
-    <col min="107" max="107" width="10.6719" style="1" customWidth="1"/>
-    <col min="108" max="108" width="10.6719" style="1" customWidth="1"/>
-    <col min="109" max="109" width="10.6719" style="1" customWidth="1"/>
-    <col min="110" max="110" width="10.6719" style="1" customWidth="1"/>
-    <col min="111" max="111" width="10.6719" style="1" customWidth="1"/>
-    <col min="112" max="112" width="10.6719" style="1" customWidth="1"/>
-    <col min="113" max="113" width="10.6719" style="1" customWidth="1"/>
-    <col min="114" max="114" width="10.6719" style="1" customWidth="1"/>
-    <col min="115" max="115" width="10.6719" style="1" customWidth="1"/>
-    <col min="116" max="116" width="10.6719" style="1" customWidth="1"/>
-    <col min="117" max="117" width="10.6719" style="1" customWidth="1"/>
-    <col min="118" max="118" width="10.6719" style="1" customWidth="1"/>
-    <col min="119" max="119" width="10.6719" style="1" customWidth="1"/>
-    <col min="120" max="120" width="10.6719" style="1" customWidth="1"/>
-    <col min="121" max="121" width="10.6719" style="1" customWidth="1"/>
-    <col min="122" max="122" width="10.6719" style="1" customWidth="1"/>
-    <col min="123" max="123" width="10.6719" style="1" customWidth="1"/>
-    <col min="124" max="124" width="10.6719" style="1" customWidth="1"/>
-    <col min="125" max="125" width="10.6719" style="1" customWidth="1"/>
-    <col min="126" max="126" width="10.6719" style="1" customWidth="1"/>
-    <col min="127" max="127" width="10.6719" style="1" customWidth="1"/>
-    <col min="128" max="128" width="10.6719" style="1" customWidth="1"/>
-    <col min="129" max="129" width="10.6719" style="1" customWidth="1"/>
-    <col min="130" max="130" width="10.6719" style="1" customWidth="1"/>
-    <col min="131" max="131" width="10.6719" style="1" customWidth="1"/>
-    <col min="132" max="132" width="10.6719" style="1" customWidth="1"/>
-    <col min="133" max="133" width="10.6719" style="1" customWidth="1"/>
-    <col min="134" max="134" width="10.6719" style="1" customWidth="1"/>
-    <col min="135" max="135" width="10.6719" style="1" customWidth="1"/>
-    <col min="136" max="136" width="10.6719" style="1" customWidth="1"/>
-    <col min="137" max="137" width="10.6719" style="1" customWidth="1"/>
-    <col min="138" max="138" width="10.6719" style="1" customWidth="1"/>
-    <col min="139" max="139" width="10.6719" style="1" customWidth="1"/>
-    <col min="140" max="140" width="10.6719" style="1" customWidth="1"/>
-    <col min="141" max="141" width="10.6719" style="1" customWidth="1"/>
-    <col min="142" max="142" width="10.6719" style="1" customWidth="1"/>
-    <col min="143" max="143" width="10.6719" style="1" customWidth="1"/>
-    <col min="144" max="144" width="10.6719" style="1" customWidth="1"/>
-    <col min="145" max="145" width="10.6719" style="1" customWidth="1"/>
-    <col min="146" max="146" width="10.6719" style="1" customWidth="1"/>
-    <col min="147" max="147" width="10.6719" style="1" customWidth="1"/>
-    <col min="148" max="148" width="10.6719" style="1" customWidth="1"/>
-    <col min="149" max="149" width="10.6719" style="1" customWidth="1"/>
-    <col min="150" max="150" width="10.6719" style="1" customWidth="1"/>
-    <col min="151" max="151" width="10.6719" style="1" customWidth="1"/>
-    <col min="152" max="152" width="10.6719" style="1" customWidth="1"/>
-    <col min="153" max="153" width="10.6719" style="1" customWidth="1"/>
-    <col min="154" max="154" width="10.6719" style="1" customWidth="1"/>
-    <col min="155" max="155" width="10.6719" style="1" customWidth="1"/>
-    <col min="156" max="156" width="10.6719" style="1" customWidth="1"/>
-    <col min="157" max="157" width="10.6719" style="1" customWidth="1"/>
-    <col min="158" max="158" width="10.6719" style="1" customWidth="1"/>
-    <col min="159" max="159" width="10.6719" style="1" customWidth="1"/>
-    <col min="160" max="160" width="10.6719" style="1" customWidth="1"/>
-    <col min="161" max="161" width="10.6719" style="1" customWidth="1"/>
-    <col min="162" max="162" width="10.6719" style="1" customWidth="1"/>
-    <col min="163" max="163" width="10.6719" style="1" customWidth="1"/>
-    <col min="164" max="164" width="10.6719" style="1" customWidth="1"/>
-    <col min="165" max="165" width="10.6719" style="1" customWidth="1"/>
-    <col min="166" max="166" width="10.6719" style="1" customWidth="1"/>
-    <col min="167" max="167" width="10.6719" style="1" customWidth="1"/>
-    <col min="168" max="168" width="10.6719" style="1" customWidth="1"/>
-    <col min="169" max="169" width="10.6719" style="1" customWidth="1"/>
-    <col min="170" max="170" width="10.6719" style="1" customWidth="1"/>
-    <col min="171" max="171" width="10.6719" style="1" customWidth="1"/>
-    <col min="172" max="172" width="10.6719" style="1" customWidth="1"/>
-    <col min="173" max="173" width="10.6719" style="1" customWidth="1"/>
-    <col min="174" max="174" width="10.6719" style="1" customWidth="1"/>
-    <col min="175" max="175" width="10.6719" style="1" customWidth="1"/>
-    <col min="176" max="176" width="10.6719" style="1" customWidth="1"/>
-    <col min="177" max="177" width="10.6719" style="1" customWidth="1"/>
-    <col min="178" max="178" width="10.6719" style="1" customWidth="1"/>
-    <col min="179" max="179" width="10.6719" style="1" customWidth="1"/>
-    <col min="180" max="180" width="10.6719" style="1" customWidth="1"/>
-    <col min="181" max="181" width="10.6719" style="1" customWidth="1"/>
-    <col min="182" max="182" width="10.6719" style="1" customWidth="1"/>
-    <col min="183" max="183" width="10.6719" style="1" customWidth="1"/>
-    <col min="184" max="184" width="10.6719" style="1" customWidth="1"/>
-    <col min="185" max="185" width="10.6719" style="1" customWidth="1"/>
-    <col min="186" max="186" width="10.6719" style="1" customWidth="1"/>
-    <col min="187" max="187" width="10.6719" style="1" customWidth="1"/>
-    <col min="188" max="188" width="10.6719" style="1" customWidth="1"/>
-    <col min="189" max="189" width="10.6719" style="1" customWidth="1"/>
-    <col min="190" max="190" width="10.6719" style="1" customWidth="1"/>
-    <col min="191" max="191" width="10.6719" style="1" customWidth="1"/>
-    <col min="192" max="192" width="10.6719" style="1" customWidth="1"/>
-    <col min="193" max="193" width="10.6719" style="1" customWidth="1"/>
-    <col min="194" max="194" width="10.6719" style="1" customWidth="1"/>
-    <col min="195" max="195" width="10.6719" style="1" customWidth="1"/>
-    <col min="196" max="196" width="10.6719" style="1" customWidth="1"/>
-    <col min="197" max="197" width="10.6719" style="1" customWidth="1"/>
-    <col min="198" max="198" width="10.6719" style="1" customWidth="1"/>
-    <col min="199" max="199" width="10.6719" style="1" customWidth="1"/>
-    <col min="200" max="200" width="10.6719" style="1" customWidth="1"/>
-    <col min="201" max="201" width="10.6719" style="1" customWidth="1"/>
-    <col min="202" max="202" width="10.6719" style="1" customWidth="1"/>
-    <col min="203" max="203" width="10.6719" style="1" customWidth="1"/>
-    <col min="204" max="204" width="10.6719" style="1" customWidth="1"/>
-    <col min="205" max="205" width="10.6719" style="1" customWidth="1"/>
-    <col min="206" max="206" width="10.6719" style="1" customWidth="1"/>
-    <col min="207" max="207" width="10.6719" style="1" customWidth="1"/>
-    <col min="208" max="208" width="10.6719" style="1" customWidth="1"/>
-    <col min="209" max="209" width="10.6719" style="1" customWidth="1"/>
-    <col min="210" max="210" width="10.6719" style="1" customWidth="1"/>
-    <col min="211" max="211" width="10.6719" style="1" customWidth="1"/>
-    <col min="212" max="212" width="10.6719" style="1" customWidth="1"/>
-    <col min="213" max="213" width="10.6719" style="1" customWidth="1"/>
-    <col min="214" max="214" width="10.6719" style="1" customWidth="1"/>
-    <col min="215" max="215" width="10.6719" style="1" customWidth="1"/>
-    <col min="216" max="216" width="10.6719" style="1" customWidth="1"/>
-    <col min="217" max="217" width="10.6719" style="1" customWidth="1"/>
-    <col min="218" max="218" width="10.6719" style="1" customWidth="1"/>
-    <col min="219" max="219" width="10.6719" style="1" customWidth="1"/>
-    <col min="220" max="220" width="10.6719" style="1" customWidth="1"/>
-    <col min="221" max="221" width="10.6719" style="1" customWidth="1"/>
-    <col min="222" max="222" width="10.6719" style="1" customWidth="1"/>
-    <col min="223" max="223" width="10.6719" style="1" customWidth="1"/>
-    <col min="224" max="224" width="10.6719" style="1" customWidth="1"/>
-    <col min="225" max="225" width="10.6719" style="1" customWidth="1"/>
-    <col min="226" max="226" width="10.6719" style="1" customWidth="1"/>
-    <col min="227" max="227" width="10.6719" style="1" customWidth="1"/>
-    <col min="228" max="228" width="10.6719" style="1" customWidth="1"/>
-    <col min="229" max="229" width="10.6719" style="1" customWidth="1"/>
-    <col min="230" max="230" width="10.6719" style="1" customWidth="1"/>
-    <col min="231" max="231" width="10.6719" style="1" customWidth="1"/>
-    <col min="232" max="232" width="10.6719" style="1" customWidth="1"/>
-    <col min="233" max="233" width="10.6719" style="1" customWidth="1"/>
-    <col min="234" max="234" width="10.6719" style="1" customWidth="1"/>
-    <col min="235" max="235" width="10.6719" style="1" customWidth="1"/>
-    <col min="236" max="236" width="10.6719" style="1" customWidth="1"/>
-    <col min="237" max="237" width="10.6719" style="1" customWidth="1"/>
-    <col min="238" max="238" width="10.6719" style="1" customWidth="1"/>
-    <col min="239" max="239" width="10.6719" style="1" customWidth="1"/>
-    <col min="240" max="240" width="10.6719" style="1" customWidth="1"/>
-    <col min="241" max="241" width="10.6719" style="1" customWidth="1"/>
-    <col min="242" max="242" width="10.6719" style="1" customWidth="1"/>
-    <col min="243" max="243" width="10.6719" style="1" customWidth="1"/>
-    <col min="244" max="244" width="10.6719" style="1" customWidth="1"/>
-    <col min="245" max="245" width="10.6719" style="1" customWidth="1"/>
-    <col min="246" max="246" width="10.6719" style="1" customWidth="1"/>
-    <col min="247" max="247" width="10.6719" style="1" customWidth="1"/>
-    <col min="248" max="248" width="10.6719" style="1" customWidth="1"/>
-    <col min="249" max="249" width="10.6719" style="1" customWidth="1"/>
-    <col min="250" max="250" width="10.6719" style="1" customWidth="1"/>
-    <col min="251" max="251" width="10.6719" style="1" customWidth="1"/>
-    <col min="252" max="252" width="10.6719" style="1" customWidth="1"/>
-    <col min="253" max="253" width="10.6719" style="1" customWidth="1"/>
-    <col min="254" max="254" width="10.6719" style="1" customWidth="1"/>
-    <col min="255" max="255" width="10.6719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="69.6640625" style="1" customWidth="1"/>
+    <col min="6" max="255" width="10.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:255" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3"/>
@@ -2246,17 +2044,17 @@
       <c r="IT1" s="4"/>
       <c r="IU1" s="5"/>
     </row>
-    <row r="2" ht="15" customHeight="1">
+    <row r="2" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="7">
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="8"/>
@@ -2511,17 +2309,17 @@
       <c r="IT2" s="10"/>
       <c r="IU2" s="11"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="13">
+      <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="13">
+      <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s" s="13">
+      <c r="D3" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="14"/>
@@ -2776,17 +2574,17 @@
       <c r="IT3" s="10"/>
       <c r="IU3" s="11"/>
     </row>
-    <row r="4" ht="29" customHeight="1">
+    <row r="4" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s" s="7">
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="7">
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="8"/>
@@ -3041,17 +2839,17 @@
       <c r="IT4" s="10"/>
       <c r="IU4" s="11"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="13">
+      <c r="B5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s" s="13">
+      <c r="C5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s" s="13">
+      <c r="D5" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="14"/>
@@ -3306,17 +3104,17 @@
       <c r="IT5" s="10"/>
       <c r="IU5" s="11"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="7">
+      <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s" s="7">
+      <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s" s="7">
+      <c r="D6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="8"/>
@@ -3571,17 +3369,17 @@
       <c r="IT6" s="10"/>
       <c r="IU6" s="11"/>
     </row>
-    <row r="7" ht="29" customHeight="1">
+    <row r="7" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="13">
+      <c r="B7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s" s="13">
+      <c r="C7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s" s="13">
+      <c r="D7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="14"/>
@@ -3836,17 +3634,17 @@
       <c r="IT7" s="10"/>
       <c r="IU7" s="11"/>
     </row>
-    <row r="8" ht="29" customHeight="1">
+    <row r="8" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="7">
+      <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s" s="7">
+      <c r="C8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s" s="7">
+      <c r="D8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="8"/>
@@ -4101,17 +3899,17 @@
       <c r="IT8" s="10"/>
       <c r="IU8" s="11"/>
     </row>
-    <row r="9" ht="29" customHeight="1">
+    <row r="9" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="13">
+      <c r="B9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s" s="13">
+      <c r="C9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s" s="13">
+      <c r="D9" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="14"/>
@@ -4366,17 +4164,17 @@
       <c r="IT9" s="10"/>
       <c r="IU9" s="11"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="7">
+      <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s" s="7">
+      <c r="C10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s" s="7">
+      <c r="D10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="8"/>
@@ -4631,17 +4429,17 @@
       <c r="IT10" s="10"/>
       <c r="IU10" s="11"/>
     </row>
-    <row r="11" ht="15" customHeight="1">
+    <row r="11" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="13">
+      <c r="B11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s" s="13">
+      <c r="C11" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D11" t="s" s="13">
+      <c r="D11" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="14"/>
@@ -4896,17 +4694,17 @@
       <c r="IT11" s="10"/>
       <c r="IU11" s="11"/>
     </row>
-    <row r="12" ht="15" customHeight="1">
+    <row r="12" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" t="s" s="7">
+      <c r="B12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s" s="7">
+      <c r="C12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D12" t="s" s="7">
+      <c r="D12" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="8"/>
@@ -5161,17 +4959,17 @@
       <c r="IT12" s="10"/>
       <c r="IU12" s="11"/>
     </row>
-    <row r="13" ht="15" customHeight="1">
+    <row r="13" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>12</v>
       </c>
-      <c r="B13" t="s" s="13">
+      <c r="B13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s" s="13">
+      <c r="C13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D13" t="s" s="13">
+      <c r="D13" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="14"/>
@@ -5426,17 +5224,17 @@
       <c r="IT13" s="10"/>
       <c r="IU13" s="11"/>
     </row>
-    <row r="14" ht="15" customHeight="1">
+    <row r="14" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" t="s" s="7">
+      <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C14" t="s" s="7">
+      <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D14" t="s" s="7">
+      <c r="D14" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="8"/>
@@ -5691,17 +5489,17 @@
       <c r="IT14" s="10"/>
       <c r="IU14" s="11"/>
     </row>
-    <row r="15" ht="15" customHeight="1">
+    <row r="15" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>14</v>
       </c>
-      <c r="B15" t="s" s="13">
+      <c r="B15" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C15" t="s" s="13">
+      <c r="C15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D15" t="s" s="13">
+      <c r="D15" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="14"/>
@@ -5956,17 +5754,17 @@
       <c r="IT15" s="10"/>
       <c r="IU15" s="11"/>
     </row>
-    <row r="16" ht="31" customHeight="1">
+    <row r="16" spans="1:255" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" t="s" s="7">
+      <c r="B16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="s" s="7">
+      <c r="C16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D16" t="s" s="7">
+      <c r="D16" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="8"/>
@@ -6221,17 +6019,17 @@
       <c r="IT16" s="10"/>
       <c r="IU16" s="11"/>
     </row>
-    <row r="17" ht="29" customHeight="1">
+    <row r="17" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>16</v>
       </c>
-      <c r="B17" t="s" s="13">
+      <c r="B17" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C17" t="s" s="13">
+      <c r="C17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D17" t="s" s="13">
+      <c r="D17" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="14"/>
@@ -6486,17 +6284,17 @@
       <c r="IT17" s="10"/>
       <c r="IU17" s="11"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
+    <row r="18" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" t="s" s="7">
+      <c r="B18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C18" t="s" s="7">
+      <c r="C18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D18" t="s" s="7">
+      <c r="D18" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="8"/>
@@ -6751,17 +6549,17 @@
       <c r="IT18" s="10"/>
       <c r="IU18" s="11"/>
     </row>
-    <row r="19" ht="15" customHeight="1">
+    <row r="19" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>18</v>
       </c>
-      <c r="B19" t="s" s="13">
+      <c r="B19" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C19" t="s" s="13">
+      <c r="C19" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="s" s="13">
+      <c r="D19" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="14"/>
@@ -7016,17 +6814,17 @@
       <c r="IT19" s="10"/>
       <c r="IU19" s="11"/>
     </row>
-    <row r="20" ht="29" customHeight="1">
+    <row r="20" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" t="s" s="7">
+      <c r="B20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C20" t="s" s="7">
+      <c r="C20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D20" t="s" s="7">
+      <c r="D20" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="8"/>
@@ -7281,17 +7079,17 @@
       <c r="IT20" s="10"/>
       <c r="IU20" s="11"/>
     </row>
-    <row r="21" ht="29" customHeight="1">
+    <row r="21" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>20</v>
       </c>
-      <c r="B21" t="s" s="13">
+      <c r="B21" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C21" t="s" s="13">
+      <c r="C21" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D21" t="s" s="13">
+      <c r="D21" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="14"/>
@@ -7546,17 +7344,17 @@
       <c r="IT21" s="10"/>
       <c r="IU21" s="11"/>
     </row>
-    <row r="22" ht="29" customHeight="1">
+    <row r="22" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="B22" t="s" s="7">
+      <c r="B22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C22" t="s" s="7">
+      <c r="C22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D22" t="s" s="7">
+      <c r="D22" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="8"/>
@@ -7811,17 +7609,17 @@
       <c r="IT22" s="10"/>
       <c r="IU22" s="11"/>
     </row>
-    <row r="23" ht="29" customHeight="1">
+    <row r="23" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>22</v>
       </c>
-      <c r="B23" t="s" s="13">
+      <c r="B23" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C23" t="s" s="13">
+      <c r="C23" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D23" t="s" s="13">
+      <c r="D23" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="14"/>
@@ -8076,17 +7874,17 @@
       <c r="IT23" s="10"/>
       <c r="IU23" s="11"/>
     </row>
-    <row r="24" ht="29" customHeight="1">
+    <row r="24" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" t="s" s="7">
+      <c r="B24" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C24" t="s" s="7">
+      <c r="C24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D24" t="s" s="7">
+      <c r="D24" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="8"/>
@@ -8341,17 +8139,17 @@
       <c r="IT24" s="10"/>
       <c r="IU24" s="11"/>
     </row>
-    <row r="25" ht="16" customHeight="1">
+    <row r="25" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>24</v>
       </c>
-      <c r="B25" t="s" s="13">
+      <c r="B25" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C25" t="s" s="13">
+      <c r="C25" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D25" t="s" s="13">
+      <c r="D25" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E25" s="14"/>
@@ -8606,14 +8404,14 @@
       <c r="IT25" s="10"/>
       <c r="IU25" s="11"/>
     </row>
-    <row r="26" ht="16" customHeight="1">
+    <row r="26" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" t="s" s="7">
+      <c r="B26" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C26" t="s" s="7">
+      <c r="C26" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D26" s="8"/>
@@ -8869,14 +8667,14 @@
       <c r="IT26" s="10"/>
       <c r="IU26" s="11"/>
     </row>
-    <row r="27" ht="16" customHeight="1">
+    <row r="27" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>26</v>
       </c>
-      <c r="B27" t="s" s="13">
+      <c r="B27" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C27" t="s" s="13">
+      <c r="C27" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D27" s="14"/>
@@ -9132,14 +8930,14 @@
       <c r="IT27" s="10"/>
       <c r="IU27" s="11"/>
     </row>
-    <row r="28" ht="16" customHeight="1">
+    <row r="28" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="B28" t="s" s="7">
+      <c r="B28" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C28" t="s" s="7">
+      <c r="C28" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="8"/>
@@ -9395,18 +9193,18 @@
       <c r="IT28" s="10"/>
       <c r="IU28" s="11"/>
     </row>
-    <row r="29" ht="15" customHeight="1">
+    <row r="29" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>28</v>
       </c>
-      <c r="B29" t="s" s="13">
+      <c r="B29" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C29" t="s" s="13">
+      <c r="C29" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D29" s="14"/>
-      <c r="E29" t="s" s="13">
+      <c r="E29" s="13" t="s">
         <v>40</v>
       </c>
       <c r="F29" s="9"/>
@@ -9660,14 +9458,14 @@
       <c r="IT29" s="10"/>
       <c r="IU29" s="11"/>
     </row>
-    <row r="30" ht="16" customHeight="1">
+    <row r="30" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>29</v>
       </c>
-      <c r="B30" t="s" s="7">
+      <c r="B30" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C30" t="s" s="7">
+      <c r="C30" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="8"/>
@@ -9923,14 +9721,14 @@
       <c r="IT30" s="10"/>
       <c r="IU30" s="11"/>
     </row>
-    <row r="31" ht="32" customHeight="1">
+    <row r="31" spans="1:255" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>30</v>
       </c>
-      <c r="B31" t="s" s="13">
+      <c r="B31" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C31" t="s" s="13">
+      <c r="C31" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="14"/>
@@ -10186,18 +9984,18 @@
       <c r="IT31" s="10"/>
       <c r="IU31" s="11"/>
     </row>
-    <row r="32" ht="32" customHeight="1">
+    <row r="32" spans="1:255" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>31</v>
       </c>
-      <c r="B32" t="s" s="7">
+      <c r="B32" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C32" t="s" s="7">
+      <c r="C32" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D32" s="8"/>
-      <c r="E32" t="s" s="7">
+      <c r="E32" s="7" t="s">
         <v>44</v>
       </c>
       <c r="F32" s="9"/>
@@ -10451,18 +10249,18 @@
       <c r="IT32" s="10"/>
       <c r="IU32" s="11"/>
     </row>
-    <row r="33" ht="16" customHeight="1">
+    <row r="33" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>32</v>
       </c>
-      <c r="B33" t="s" s="13">
+      <c r="B33" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C33" t="s" s="13">
+      <c r="C33" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D33" s="14"/>
-      <c r="E33" t="s" s="13">
+      <c r="E33" s="13" t="s">
         <v>46</v>
       </c>
       <c r="F33" s="9"/>
@@ -10716,14 +10514,14 @@
       <c r="IT33" s="10"/>
       <c r="IU33" s="11"/>
     </row>
-    <row r="34" ht="15" customHeight="1">
+    <row r="34" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>33</v>
       </c>
-      <c r="B34" t="s" s="7">
+      <c r="B34" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C34" t="s" s="7">
+      <c r="C34" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D34" s="8"/>
@@ -10979,14 +10777,14 @@
       <c r="IT34" s="10"/>
       <c r="IU34" s="11"/>
     </row>
-    <row r="35" ht="15" customHeight="1">
+    <row r="35" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>34</v>
       </c>
-      <c r="B35" t="s" s="13">
+      <c r="B35" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C35" t="s" s="13">
+      <c r="C35" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D35" s="13"/>
@@ -11242,14 +11040,14 @@
       <c r="IT35" s="10"/>
       <c r="IU35" s="11"/>
     </row>
-    <row r="36" ht="15" customHeight="1">
+    <row r="36" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="12">
         <v>35</v>
       </c>
-      <c r="B36" t="s" s="7">
+      <c r="B36" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C36" t="s" s="7">
+      <c r="C36" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="7"/>
@@ -11505,20 +11303,20 @@
       <c r="IT36" s="10"/>
       <c r="IU36" s="11"/>
     </row>
-    <row r="37" ht="15" customHeight="1">
+    <row r="37" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12">
         <v>36</v>
       </c>
-      <c r="B37" t="s" s="13">
+      <c r="B37" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C37" t="s" s="13">
+      <c r="C37" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D37" t="s" s="13">
+      <c r="D37" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E37" t="s" s="13">
+      <c r="E37" s="13" t="s">
         <v>51</v>
       </c>
       <c r="F37" s="9"/>
@@ -11772,20 +11570,20 @@
       <c r="IT37" s="10"/>
       <c r="IU37" s="11"/>
     </row>
-    <row r="38" ht="15" customHeight="1">
+    <row r="38" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
         <v>37</v>
       </c>
-      <c r="B38" t="s" s="7">
+      <c r="B38" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C38" t="s" s="7">
+      <c r="C38" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D38" t="s" s="7">
+      <c r="D38" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E38" t="s" s="7">
+      <c r="E38" s="7" t="s">
         <v>53</v>
       </c>
       <c r="F38" s="9"/>
@@ -12039,17 +11837,17 @@
       <c r="IT38" s="10"/>
       <c r="IU38" s="11"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:255" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12">
         <v>38</v>
       </c>
-      <c r="B39" t="s" s="13">
+      <c r="B39" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C39" t="s" s="13">
+      <c r="C39" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D39" t="s" s="13">
+      <c r="D39" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E39" s="14"/>
@@ -12304,17 +12102,17 @@
       <c r="IT39" s="10"/>
       <c r="IU39" s="11"/>
     </row>
-    <row r="40" ht="15" customHeight="1">
+    <row r="40" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="12">
         <v>39</v>
       </c>
-      <c r="B40" t="s" s="7">
+      <c r="B40" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C40" t="s" s="7">
+      <c r="C40" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D40" t="s" s="7">
+      <c r="D40" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E40" s="8"/>
@@ -12569,17 +12367,17 @@
       <c r="IT40" s="10"/>
       <c r="IU40" s="11"/>
     </row>
-    <row r="41" ht="15" customHeight="1">
+    <row r="41" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="6">
         <v>40</v>
       </c>
-      <c r="B41" t="s" s="13">
+      <c r="B41" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C41" t="s" s="13">
+      <c r="C41" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D41" t="s" s="13">
+      <c r="D41" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E41" s="14"/>
@@ -12834,17 +12632,17 @@
       <c r="IT41" s="10"/>
       <c r="IU41" s="11"/>
     </row>
-    <row r="42" ht="15" customHeight="1">
+    <row r="42" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="12">
         <v>41</v>
       </c>
-      <c r="B42" t="s" s="7">
+      <c r="B42" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C42" t="s" s="7">
+      <c r="C42" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D42" t="s" s="7">
+      <c r="D42" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E42" s="8"/>
@@ -13099,17 +12897,17 @@
       <c r="IT42" s="10"/>
       <c r="IU42" s="11"/>
     </row>
-    <row r="43" ht="15" customHeight="1">
+    <row r="43" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="12">
         <v>42</v>
       </c>
-      <c r="B43" t="s" s="13">
+      <c r="B43" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C43" t="s" s="13">
+      <c r="C43" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D43" t="s" s="13">
+      <c r="D43" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E43" s="14"/>
@@ -13364,17 +13162,17 @@
       <c r="IT43" s="10"/>
       <c r="IU43" s="11"/>
     </row>
-    <row r="44" ht="15" customHeight="1">
+    <row r="44" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
         <v>43</v>
       </c>
-      <c r="B44" t="s" s="7">
+      <c r="B44" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C44" t="s" s="7">
+      <c r="C44" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D44" t="s" s="7">
+      <c r="D44" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E44" s="8"/>
@@ -13629,17 +13427,17 @@
       <c r="IT44" s="10"/>
       <c r="IU44" s="11"/>
     </row>
-    <row r="45" ht="15" customHeight="1">
+    <row r="45" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="12">
         <v>44</v>
       </c>
-      <c r="B45" t="s" s="13">
+      <c r="B45" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C45" t="s" s="13">
+      <c r="C45" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D45" t="s" s="13">
+      <c r="D45" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E45" s="14"/>
@@ -13894,14 +13692,14 @@
       <c r="IT45" s="10"/>
       <c r="IU45" s="11"/>
     </row>
-    <row r="46" ht="15" customHeight="1">
+    <row r="46" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="12">
         <v>45</v>
       </c>
-      <c r="B46" t="s" s="7">
+      <c r="B46" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C46" t="s" s="7">
+      <c r="C46" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D46" s="8"/>
@@ -14157,17 +13955,17 @@
       <c r="IT46" s="10"/>
       <c r="IU46" s="11"/>
     </row>
-    <row r="47" ht="15" customHeight="1">
+    <row r="47" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
         <v>46</v>
       </c>
-      <c r="B47" t="s" s="13">
+      <c r="B47" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C47" t="s" s="13">
+      <c r="C47" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D47" t="s" s="13">
+      <c r="D47" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="14"/>
@@ -14422,14 +14220,14 @@
       <c r="IT47" s="10"/>
       <c r="IU47" s="11"/>
     </row>
-    <row r="48" ht="15" customHeight="1">
+    <row r="48" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="12">
         <v>47</v>
       </c>
-      <c r="B48" t="s" s="7">
+      <c r="B48" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C48" t="s" s="7">
+      <c r="C48" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D48" s="8"/>
@@ -14685,17 +14483,17 @@
       <c r="IT48" s="10"/>
       <c r="IU48" s="11"/>
     </row>
-    <row r="49" ht="15" customHeight="1">
+    <row r="49" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="12">
         <v>48</v>
       </c>
-      <c r="B49" t="s" s="13">
+      <c r="B49" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C49" t="s" s="13">
+      <c r="C49" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D49" t="s" s="13">
+      <c r="D49" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E49" s="14"/>
@@ -14950,17 +14748,17 @@
       <c r="IT49" s="10"/>
       <c r="IU49" s="11"/>
     </row>
-    <row r="50" ht="15" customHeight="1">
+    <row r="50" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
         <v>49</v>
       </c>
-      <c r="B50" t="s" s="7">
+      <c r="B50" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C50" t="s" s="7">
+      <c r="C50" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D50" t="s" s="7">
+      <c r="D50" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E50" s="8"/>
@@ -15215,17 +15013,17 @@
       <c r="IT50" s="10"/>
       <c r="IU50" s="11"/>
     </row>
-    <row r="51" ht="15" customHeight="1">
+    <row r="51" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="12">
         <v>50</v>
       </c>
-      <c r="B51" t="s" s="13">
+      <c r="B51" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C51" t="s" s="13">
+      <c r="C51" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D51" t="s" s="13">
+      <c r="D51" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E51" s="14"/>
@@ -15480,17 +15278,17 @@
       <c r="IT51" s="10"/>
       <c r="IU51" s="11"/>
     </row>
-    <row r="52" ht="15" customHeight="1">
+    <row r="52" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="12">
         <v>51</v>
       </c>
-      <c r="B52" t="s" s="7">
+      <c r="B52" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C52" t="s" s="7">
+      <c r="C52" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D52" t="s" s="7">
+      <c r="D52" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E52" s="8"/>
@@ -15745,17 +15543,17 @@
       <c r="IT52" s="10"/>
       <c r="IU52" s="11"/>
     </row>
-    <row r="53" ht="31.25" customHeight="1">
+    <row r="53" spans="1:255" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
         <v>52</v>
       </c>
-      <c r="B53" t="s" s="13">
+      <c r="B53" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C53" t="s" s="13">
+      <c r="C53" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D53" t="s" s="13">
+      <c r="D53" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E53" s="14"/>
@@ -16010,17 +15808,17 @@
       <c r="IT53" s="10"/>
       <c r="IU53" s="11"/>
     </row>
-    <row r="54" ht="31.25" customHeight="1">
+    <row r="54" spans="1:255" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="12">
         <v>53</v>
       </c>
-      <c r="B54" t="s" s="7">
+      <c r="B54" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C54" t="s" s="7">
+      <c r="C54" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D54" t="s" s="7">
+      <c r="D54" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E54" s="8"/>
@@ -16275,17 +16073,17 @@
       <c r="IT54" s="10"/>
       <c r="IU54" s="11"/>
     </row>
-    <row r="55" ht="31.25" customHeight="1">
+    <row r="55" spans="1:255" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="12">
         <v>54</v>
       </c>
-      <c r="B55" t="s" s="13">
+      <c r="B55" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C55" t="s" s="13">
+      <c r="C55" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D55" t="s" s="13">
+      <c r="D55" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E55" s="14"/>
@@ -16540,17 +16338,17 @@
       <c r="IT55" s="10"/>
       <c r="IU55" s="11"/>
     </row>
-    <row r="56" ht="18.75" customHeight="1">
+    <row r="56" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
         <v>55</v>
       </c>
-      <c r="B56" t="s" s="7">
+      <c r="B56" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C56" t="s" s="7">
+      <c r="C56" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D56" t="s" s="7">
+      <c r="D56" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E56" s="8"/>
@@ -16805,17 +16603,17 @@
       <c r="IT56" s="10"/>
       <c r="IU56" s="11"/>
     </row>
-    <row r="57" ht="18.75" customHeight="1">
+    <row r="57" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="12">
         <v>56</v>
       </c>
-      <c r="B57" t="s" s="13">
+      <c r="B57" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C57" t="s" s="13">
+      <c r="C57" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D57" t="s" s="13">
+      <c r="D57" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E57" s="14"/>
@@ -17070,14 +16868,14 @@
       <c r="IT57" s="10"/>
       <c r="IU57" s="11"/>
     </row>
-    <row r="58" ht="18.75" customHeight="1">
+    <row r="58" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="12">
         <v>57</v>
       </c>
-      <c r="B58" t="s" s="7">
+      <c r="B58" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C58" t="s" s="7">
+      <c r="C58" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D58" s="8"/>
@@ -17333,14 +17131,14 @@
       <c r="IT58" s="10"/>
       <c r="IU58" s="11"/>
     </row>
-    <row r="59" ht="18.75" customHeight="1">
+    <row r="59" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
         <v>58</v>
       </c>
-      <c r="B59" t="s" s="13">
+      <c r="B59" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C59" t="s" s="13">
+      <c r="C59" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D59" s="14"/>
@@ -17596,17 +17394,17 @@
       <c r="IT59" s="10"/>
       <c r="IU59" s="11"/>
     </row>
-    <row r="60" ht="18.75" customHeight="1">
+    <row r="60" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="12">
         <v>59</v>
       </c>
-      <c r="B60" t="s" s="7">
+      <c r="B60" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C60" t="s" s="7">
+      <c r="C60" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D60" t="s" s="7">
+      <c r="D60" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E60" s="8"/>
@@ -17861,7 +17659,7 @@
       <c r="IT60" s="10"/>
       <c r="IU60" s="11"/>
     </row>
-    <row r="61" ht="18.75" customHeight="1">
+    <row r="61" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
@@ -18118,7 +17916,7 @@
       <c r="IT61" s="10"/>
       <c r="IU61" s="11"/>
     </row>
-    <row r="62" ht="18.75" customHeight="1">
+    <row r="62" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -18375,7 +18173,7 @@
       <c r="IT62" s="10"/>
       <c r="IU62" s="11"/>
     </row>
-    <row r="63" ht="18.75" customHeight="1">
+    <row r="63" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
@@ -18632,7 +18430,7 @@
       <c r="IT63" s="10"/>
       <c r="IU63" s="11"/>
     </row>
-    <row r="64" ht="18.75" customHeight="1">
+    <row r="64" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -18889,7 +18687,7 @@
       <c r="IT64" s="10"/>
       <c r="IU64" s="11"/>
     </row>
-    <row r="65" ht="18.75" customHeight="1">
+    <row r="65" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="14"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
@@ -19146,7 +18944,7 @@
       <c r="IT65" s="10"/>
       <c r="IU65" s="11"/>
     </row>
-    <row r="66" ht="18.75" customHeight="1">
+    <row r="66" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="14"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
@@ -19403,7 +19201,7 @@
       <c r="IT66" s="10"/>
       <c r="IU66" s="11"/>
     </row>
-    <row r="67" ht="18.75" customHeight="1">
+    <row r="67" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="8"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
@@ -19660,7 +19458,7 @@
       <c r="IT67" s="10"/>
       <c r="IU67" s="11"/>
     </row>
-    <row r="68" ht="18.75" customHeight="1">
+    <row r="68" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="14"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -19917,7 +19715,7 @@
       <c r="IT68" s="10"/>
       <c r="IU68" s="11"/>
     </row>
-    <row r="69" ht="18.75" customHeight="1">
+    <row r="69" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="8"/>
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
@@ -20174,7 +19972,7 @@
       <c r="IT69" s="10"/>
       <c r="IU69" s="11"/>
     </row>
-    <row r="70" ht="18.75" customHeight="1">
+    <row r="70" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="14"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -20431,7 +20229,7 @@
       <c r="IT70" s="10"/>
       <c r="IU70" s="11"/>
     </row>
-    <row r="71" ht="18.75" customHeight="1">
+    <row r="71" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="8"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
@@ -20688,7 +20486,7 @@
       <c r="IT71" s="10"/>
       <c r="IU71" s="11"/>
     </row>
-    <row r="72" ht="14" customHeight="1">
+    <row r="72" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="15"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -20945,7 +20743,7 @@
       <c r="IT72" s="10"/>
       <c r="IU72" s="11"/>
     </row>
-    <row r="73" ht="14" customHeight="1">
+    <row r="73" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="16"/>
       <c r="B73" s="14"/>
       <c r="C73" s="14"/>
@@ -21202,7 +21000,7 @@
       <c r="IT73" s="10"/>
       <c r="IU73" s="11"/>
     </row>
-    <row r="74" ht="14" customHeight="1">
+    <row r="74" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="16"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -21459,7 +21257,7 @@
       <c r="IT74" s="10"/>
       <c r="IU74" s="11"/>
     </row>
-    <row r="75" ht="14" customHeight="1">
+    <row r="75" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="16"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
@@ -21716,7 +21514,7 @@
       <c r="IT75" s="10"/>
       <c r="IU75" s="11"/>
     </row>
-    <row r="76" ht="14" customHeight="1">
+    <row r="76" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="16"/>
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
@@ -21973,7 +21771,7 @@
       <c r="IT76" s="10"/>
       <c r="IU76" s="11"/>
     </row>
-    <row r="77" ht="14" customHeight="1">
+    <row r="77" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="16"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
@@ -22230,7 +22028,7 @@
       <c r="IT77" s="10"/>
       <c r="IU77" s="11"/>
     </row>
-    <row r="78" ht="14" customHeight="1">
+    <row r="78" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="16"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
@@ -22487,7 +22285,7 @@
       <c r="IT78" s="10"/>
       <c r="IU78" s="11"/>
     </row>
-    <row r="79" ht="14" customHeight="1">
+    <row r="79" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="16"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
@@ -22744,7 +22542,7 @@
       <c r="IT79" s="10"/>
       <c r="IU79" s="11"/>
     </row>
-    <row r="80" ht="14" customHeight="1">
+    <row r="80" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="16"/>
       <c r="B80" s="14"/>
       <c r="C80" s="14"/>
@@ -23001,7 +22799,7 @@
       <c r="IT80" s="10"/>
       <c r="IU80" s="11"/>
     </row>
-    <row r="81" ht="14" customHeight="1">
+    <row r="81" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="17"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
@@ -23260,7 +23058,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -23268,390 +23066,390 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV29"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.6719" style="21" customWidth="1"/>
-    <col min="2" max="2" width="45.8516" style="21" customWidth="1"/>
-    <col min="3" max="3" width="13.3516" style="21" customWidth="1"/>
-    <col min="4" max="4" width="12.6719" style="21" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="21" customWidth="1"/>
     <col min="5" max="5" width="38.5" style="21" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="21" customWidth="1"/>
+    <col min="6" max="256" width="8.83203125" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1">
-      <c r="A1" t="s" s="22">
+    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="22">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="22">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="22">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="22">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="16" customHeight="1">
+    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="24">
+      <c r="B2" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C2" t="s" s="24">
+      <c r="C2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="7">
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s" s="24">
+      <c r="E2" s="29" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="22">
+      <c r="B3" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C3" t="s" s="22">
+      <c r="C3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s" s="13">
+      <c r="D3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="26"/>
+      <c r="E3" s="30"/>
     </row>
-    <row r="4" ht="16" customHeight="1">
+    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="24">
+      <c r="B4" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C4" t="s" s="24">
+      <c r="C4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="7">
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="31"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="22">
+      <c r="B5" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="C5" t="s" s="22">
+      <c r="C5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s" s="13">
+      <c r="D5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="30"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="23">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="24">
+      <c r="B6" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C6" t="s" s="24">
+      <c r="C6" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s" s="7">
+      <c r="D6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="27"/>
+      <c r="E6" s="31"/>
     </row>
-    <row r="7" ht="16" customHeight="1">
+    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="22">
+      <c r="B7" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C7" t="s" s="22">
+      <c r="C7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s" s="13">
+      <c r="D7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="26"/>
+      <c r="E7" s="30"/>
     </row>
-    <row r="8" ht="18.75" customHeight="1">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="23">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="24">
+      <c r="B8" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C8" t="s" s="24">
+      <c r="C8" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s" s="7">
+      <c r="D8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="27"/>
+      <c r="E8" s="31"/>
     </row>
-    <row r="9" ht="32" customHeight="1">
+    <row r="9" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="22">
+      <c r="B9" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C9" t="s" s="22">
+      <c r="C9" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s" s="13">
+      <c r="D9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="26"/>
+      <c r="E9" s="30"/>
     </row>
-    <row r="10" ht="18.75" customHeight="1">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="24">
+      <c r="B10" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C10" t="s" s="24">
+      <c r="C10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s" s="24">
+      <c r="D10" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="27"/>
+      <c r="E10" s="31"/>
     </row>
-    <row r="11" ht="18.75" customHeight="1">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="22">
+      <c r="B11" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s" s="22">
+      <c r="C11" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s" s="22">
+      <c r="D11" s="22" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="26"/>
     </row>
-    <row r="12" ht="18.75" customHeight="1">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="23">
         <v>11</v>
       </c>
-      <c r="B12" t="s" s="24">
+      <c r="B12" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s" s="24">
+      <c r="C12" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D12" t="s" s="24">
+      <c r="D12" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="27"/>
     </row>
-    <row r="13" ht="16" customHeight="1">
+    <row r="13" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25">
         <v>12</v>
       </c>
-      <c r="B13" t="s" s="22">
+      <c r="B13" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C13" t="s" s="22">
+      <c r="C13" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D13" t="s" s="22">
+      <c r="D13" s="22" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="26"/>
     </row>
-    <row r="14" ht="16" customHeight="1">
+    <row r="14" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23">
         <v>13</v>
       </c>
-      <c r="B14" t="s" s="24">
+      <c r="B14" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C14" t="s" s="24">
+      <c r="C14" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D14" t="s" s="24">
+      <c r="D14" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="27"/>
     </row>
-    <row r="15" ht="16" customHeight="1">
+    <row r="15" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="25">
         <v>14</v>
       </c>
-      <c r="B15" t="s" s="22">
+      <c r="B15" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C15" t="s" s="22">
+      <c r="C15" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D15" t="s" s="22">
+      <c r="D15" s="22" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="26"/>
     </row>
-    <row r="16" ht="18.75" customHeight="1">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="23">
         <v>15</v>
       </c>
-      <c r="B16" t="s" s="24">
+      <c r="B16" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="C16" t="s" s="24">
+      <c r="C16" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D16" t="s" s="24">
+      <c r="D16" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="27"/>
     </row>
-    <row r="17" ht="18.75" customHeight="1">
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="25">
         <v>16</v>
       </c>
-      <c r="B17" t="s" s="22">
+      <c r="B17" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C17" t="s" s="22">
+      <c r="C17" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D17" t="s" s="22">
+      <c r="D17" s="22" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="26"/>
     </row>
-    <row r="18" ht="16" customHeight="1">
+    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="23">
         <v>17</v>
       </c>
-      <c r="B18" t="s" s="24">
+      <c r="B18" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C18" t="s" s="24">
+      <c r="C18" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D18" t="s" s="24">
+      <c r="D18" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="27"/>
     </row>
-    <row r="19" ht="16" customHeight="1">
+    <row r="19" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="25">
         <v>18</v>
       </c>
-      <c r="B19" t="s" s="22">
+      <c r="B19" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C19" t="s" s="22">
+      <c r="C19" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D19" t="s" s="22">
+      <c r="D19" s="22" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="26"/>
     </row>
-    <row r="20" ht="16" customHeight="1">
+    <row r="20" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="23">
         <v>19</v>
       </c>
-      <c r="B20" t="s" s="24">
+      <c r="B20" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C20" t="s" s="24">
+      <c r="C20" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D20" t="s" s="24">
+      <c r="D20" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="27"/>
     </row>
-    <row r="21" ht="18.75" customHeight="1">
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="25">
         <v>20</v>
       </c>
-      <c r="B21" t="s" s="22">
+      <c r="B21" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C21" t="s" s="22">
+      <c r="C21" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D21" t="s" s="22">
+      <c r="D21" s="22" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="26"/>
     </row>
-    <row r="22" ht="15" customHeight="1">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="27"/>
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
     </row>
-    <row r="23" ht="15" customHeight="1">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="26"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
     </row>
-    <row r="24" ht="15" customHeight="1">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="27"/>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
     </row>
-    <row r="25" ht="15" customHeight="1">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="26"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
     </row>
-    <row r="26" ht="15" customHeight="1">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="27"/>
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
     </row>
-    <row r="27" ht="15" customHeight="1">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="26"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
     </row>
-    <row r="28" ht="15" customHeight="1">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="27"/>
       <c r="B28" s="24"/>
       <c r="C28" s="27"/>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
     </row>
-    <row r="29" ht="15" customHeight="1">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="26"/>
       <c r="B29" s="22"/>
       <c r="C29" s="26"/>
@@ -23663,7 +23461,7 @@
     <mergeCell ref="E2:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -23671,399 +23469,401 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV32"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="28" customWidth="1"/>
-    <col min="2" max="2" width="37.3516" style="28" customWidth="1"/>
-    <col min="3" max="3" width="18.6719" style="28" customWidth="1"/>
-    <col min="4" max="4" width="11.3516" style="28" customWidth="1"/>
-    <col min="5" max="5" width="40.8516" style="28" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="28" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="28" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" style="28" customWidth="1"/>
+    <col min="6" max="256" width="8.83203125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1">
-      <c r="A1" t="s" s="13">
+    <row r="1" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="13">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="13">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="13">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="13">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="29" customHeight="1">
+    <row r="2" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>18</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s" s="7">
+      <c r="D2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" ht="32" customHeight="1">
+    <row r="3" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <v>21</v>
       </c>
-      <c r="B3" t="s" s="13">
+      <c r="B3" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C3" t="s" s="13">
+      <c r="C3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s" s="13">
+      <c r="D3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s" s="13">
+      <c r="E3" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" ht="32" customHeight="1">
+    <row r="4" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>23</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="B4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C4" t="s" s="7">
+      <c r="C4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D4" t="s" s="7">
+      <c r="D4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" ht="32" customHeight="1">
-      <c r="A5" t="s" s="13">
+    <row r="5" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B5" t="s" s="13">
+      <c r="B5" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s" s="13">
+      <c r="C5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s" s="13">
+      <c r="D5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
-      <c r="B6" t="s" s="7">
+      <c r="B6" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C6" t="s" s="7">
+      <c r="C6" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D6" t="s" s="7">
+      <c r="D6" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
-      <c r="B7" t="s" s="13">
+      <c r="B7" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C7" t="s" s="13">
+      <c r="C7" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D7" t="s" s="13">
+      <c r="D7" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
-      <c r="B8" t="s" s="7">
+      <c r="B8" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C8" t="s" s="7">
+      <c r="C8" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D8" t="s" s="7">
+      <c r="D8" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
-      <c r="B9" t="s" s="13">
+      <c r="B9" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C9" t="s" s="13">
+      <c r="C9" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D9" t="s" s="13">
+      <c r="D9" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
-      <c r="B10" t="s" s="7">
+      <c r="B10" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C10" t="s" s="7">
+      <c r="C10" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D10" t="s" s="7">
+      <c r="D10" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
-      <c r="B11" t="s" s="13">
+      <c r="B11" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C11" t="s" s="13">
+      <c r="C11" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D11" t="s" s="13">
+      <c r="D11" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="13"/>
     </row>
-    <row r="12" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
-      <c r="B12" t="s" s="7">
+      <c r="B12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C12" t="s" s="7">
+      <c r="C12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D12" t="s" s="7">
+      <c r="D12" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13"/>
-      <c r="B13" t="s" s="13">
+      <c r="B13" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C13" t="s" s="13">
+      <c r="C13" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D13" t="s" s="13">
+      <c r="D13" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="13"/>
     </row>
-    <row r="14" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
-      <c r="B14" t="s" s="7">
+      <c r="B14" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C14" t="s" s="7">
+      <c r="C14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D14" t="s" s="7">
+      <c r="D14" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" ht="32" customHeight="1">
+    <row r="15" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
-      <c r="B15" t="s" s="13">
+      <c r="B15" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C15" t="s" s="13">
+      <c r="C15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D15" t="s" s="13">
+      <c r="D15" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="13"/>
     </row>
-    <row r="16" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
-      <c r="B16" t="s" s="7">
+      <c r="B16" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C16" t="s" s="7">
+      <c r="C16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D16" t="s" s="7">
+      <c r="D16" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" ht="15" customHeight="1">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
-      <c r="B17" t="s" s="13">
+      <c r="B17" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C17" t="s" s="13">
+      <c r="C17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D17" t="s" s="13">
+      <c r="D17" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="13"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
-      <c r="B18" t="s" s="7">
+      <c r="B18" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C18" t="s" s="7">
+      <c r="C18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D18" t="s" s="7">
+      <c r="D18" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" ht="15" customHeight="1">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
-      <c r="B19" t="s" s="13">
+      <c r="B19" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C19" t="s" s="13">
+      <c r="C19" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="s" s="13">
+      <c r="D19" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="13"/>
     </row>
-    <row r="20" ht="15" customHeight="1">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
-      <c r="B20" t="s" s="7">
+      <c r="B20" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C20" t="s" s="7">
+      <c r="C20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D20" t="s" s="7">
+      <c r="D20" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" ht="15" customHeight="1">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
-      <c r="B21" t="s" s="13">
+      <c r="B21" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C21" t="s" s="13">
+      <c r="C21" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D21" t="s" s="13">
+      <c r="D21" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="13"/>
     </row>
-    <row r="22" ht="15" customHeight="1">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
-      <c r="B22" t="s" s="7">
+      <c r="B22" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C22" t="s" s="7">
+      <c r="C22" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D22" t="s" s="7">
+      <c r="D22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" ht="29" customHeight="1">
+    <row r="23" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
-      <c r="B23" t="s" s="13">
+      <c r="B23" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C23" t="s" s="13">
+      <c r="C23" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D23" t="s" s="13">
+      <c r="D23" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="13"/>
     </row>
-    <row r="24" ht="29" customHeight="1">
+    <row r="24" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
-      <c r="B24" t="s" s="7">
+      <c r="B24" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C24" t="s" s="7">
+      <c r="C24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D24" t="s" s="7">
+      <c r="D24" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" ht="15" customHeight="1">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
     </row>
-    <row r="26" ht="15" customHeight="1">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" ht="15" customHeight="1">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="14"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
     </row>
-    <row r="28" ht="15" customHeight="1">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" ht="15" customHeight="1">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
     </row>
-    <row r="30" ht="15" customHeight="1">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" ht="15" customHeight="1">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
     </row>
-    <row r="32" ht="15" customHeight="1">
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -24072,7 +23872,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updated Product Backlog, post_issue api.
</commit_message>
<xml_diff>
--- a/SSW695/product backlog.xlsx
+++ b/SSW695/product backlog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafifarab/Desktop/SSW695_Team7/SSW695/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stevens data\3rd SEM\SSW_Capstone\SSW695_Team7\SSW695\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="product backlog" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="137">
   <si>
     <t>User Story</t>
   </si>
@@ -437,11 +437,17 @@
   <si>
     <t>Edit user profile (admin portal)</t>
   </si>
+  <si>
+    <t>Create Api for post issue</t>
+  </si>
+  <si>
+    <t>Create Api to update issue</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1891,11 +1897,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IU81"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52:D54"/>
+    <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="44" style="1" customWidth="1"/>
@@ -1905,7 +1911,7 @@
     <col min="6" max="255" width="10.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:255" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2172,7 +2178,7 @@
       <c r="IT1" s="4"/>
       <c r="IU1" s="5"/>
     </row>
-    <row r="2" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2437,7 +2443,7 @@
       <c r="IT2" s="10"/>
       <c r="IU2" s="11"/>
     </row>
-    <row r="3" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -2702,7 +2708,7 @@
       <c r="IT3" s="10"/>
       <c r="IU3" s="11"/>
     </row>
-    <row r="4" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -2967,7 +2973,7 @@
       <c r="IT4" s="10"/>
       <c r="IU4" s="11"/>
     </row>
-    <row r="5" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -3232,7 +3238,7 @@
       <c r="IT5" s="10"/>
       <c r="IU5" s="11"/>
     </row>
-    <row r="6" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -3497,7 +3503,7 @@
       <c r="IT6" s="10"/>
       <c r="IU6" s="11"/>
     </row>
-    <row r="7" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -3762,7 +3768,7 @@
       <c r="IT7" s="10"/>
       <c r="IU7" s="11"/>
     </row>
-    <row r="8" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -4027,7 +4033,7 @@
       <c r="IT8" s="10"/>
       <c r="IU8" s="11"/>
     </row>
-    <row r="9" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -4292,7 +4298,7 @@
       <c r="IT9" s="10"/>
       <c r="IU9" s="11"/>
     </row>
-    <row r="10" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -4557,7 +4563,7 @@
       <c r="IT10" s="10"/>
       <c r="IU10" s="11"/>
     </row>
-    <row r="11" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -4822,7 +4828,7 @@
       <c r="IT11" s="10"/>
       <c r="IU11" s="11"/>
     </row>
-    <row r="12" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -5087,7 +5093,7 @@
       <c r="IT12" s="10"/>
       <c r="IU12" s="11"/>
     </row>
-    <row r="13" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -5352,7 +5358,7 @@
       <c r="IT13" s="10"/>
       <c r="IU13" s="11"/>
     </row>
-    <row r="14" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -5617,7 +5623,7 @@
       <c r="IT14" s="10"/>
       <c r="IU14" s="11"/>
     </row>
-    <row r="15" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -5882,7 +5888,7 @@
       <c r="IT15" s="10"/>
       <c r="IU15" s="11"/>
     </row>
-    <row r="16" spans="1:255" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:255" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -6147,7 +6153,7 @@
       <c r="IT16" s="10"/>
       <c r="IU16" s="11"/>
     </row>
-    <row r="17" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -6412,7 +6418,7 @@
       <c r="IT17" s="10"/>
       <c r="IU17" s="11"/>
     </row>
-    <row r="18" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -6677,7 +6683,7 @@
       <c r="IT18" s="10"/>
       <c r="IU18" s="11"/>
     </row>
-    <row r="19" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -6942,7 +6948,7 @@
       <c r="IT19" s="10"/>
       <c r="IU19" s="11"/>
     </row>
-    <row r="20" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -7207,7 +7213,7 @@
       <c r="IT20" s="10"/>
       <c r="IU20" s="11"/>
     </row>
-    <row r="21" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>20</v>
       </c>
@@ -7472,7 +7478,7 @@
       <c r="IT21" s="10"/>
       <c r="IU21" s="11"/>
     </row>
-    <row r="22" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -7737,7 +7743,7 @@
       <c r="IT22" s="10"/>
       <c r="IU22" s="11"/>
     </row>
-    <row r="23" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>22</v>
       </c>
@@ -8002,7 +8008,7 @@
       <c r="IT23" s="10"/>
       <c r="IU23" s="11"/>
     </row>
-    <row r="24" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:255" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -8267,7 +8273,7 @@
       <c r="IT24" s="10"/>
       <c r="IU24" s="11"/>
     </row>
-    <row r="25" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>24</v>
       </c>
@@ -8532,7 +8538,7 @@
       <c r="IT25" s="10"/>
       <c r="IU25" s="11"/>
     </row>
-    <row r="26" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -8795,7 +8801,7 @@
       <c r="IT26" s="10"/>
       <c r="IU26" s="11"/>
     </row>
-    <row r="27" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>26</v>
       </c>
@@ -9058,7 +9064,7 @@
       <c r="IT27" s="10"/>
       <c r="IU27" s="11"/>
     </row>
-    <row r="28" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -9321,7 +9327,7 @@
       <c r="IT28" s="10"/>
       <c r="IU28" s="11"/>
     </row>
-    <row r="29" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>28</v>
       </c>
@@ -9586,7 +9592,7 @@
       <c r="IT29" s="10"/>
       <c r="IU29" s="11"/>
     </row>
-    <row r="30" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -9849,7 +9855,7 @@
       <c r="IT30" s="10"/>
       <c r="IU30" s="11"/>
     </row>
-    <row r="31" spans="1:255" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:255" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>30</v>
       </c>
@@ -10112,7 +10118,7 @@
       <c r="IT31" s="10"/>
       <c r="IU31" s="11"/>
     </row>
-    <row r="32" spans="1:255" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:255" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -10377,7 +10383,7 @@
       <c r="IT32" s="10"/>
       <c r="IU32" s="11"/>
     </row>
-    <row r="33" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>32</v>
       </c>
@@ -10642,7 +10648,7 @@
       <c r="IT33" s="10"/>
       <c r="IU33" s="11"/>
     </row>
-    <row r="34" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>33</v>
       </c>
@@ -10905,7 +10911,7 @@
       <c r="IT34" s="10"/>
       <c r="IU34" s="11"/>
     </row>
-    <row r="35" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -11168,7 +11174,7 @@
       <c r="IT35" s="10"/>
       <c r="IU35" s="11"/>
     </row>
-    <row r="36" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="12">
         <v>35</v>
       </c>
@@ -11431,7 +11437,7 @@
       <c r="IT36" s="10"/>
       <c r="IU36" s="11"/>
     </row>
-    <row r="37" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12">
         <v>36</v>
       </c>
@@ -11698,7 +11704,7 @@
       <c r="IT37" s="10"/>
       <c r="IU37" s="11"/>
     </row>
-    <row r="38" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -11965,7 +11971,7 @@
       <c r="IT38" s="10"/>
       <c r="IU38" s="11"/>
     </row>
-    <row r="39" spans="1:255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:255" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12">
         <v>38</v>
       </c>
@@ -12230,7 +12236,7 @@
       <c r="IT39" s="10"/>
       <c r="IU39" s="11"/>
     </row>
-    <row r="40" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="12">
         <v>39</v>
       </c>
@@ -12495,7 +12501,7 @@
       <c r="IT40" s="10"/>
       <c r="IU40" s="11"/>
     </row>
-    <row r="41" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -12760,7 +12766,7 @@
       <c r="IT41" s="10"/>
       <c r="IU41" s="11"/>
     </row>
-    <row r="42" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="12">
         <v>41</v>
       </c>
@@ -13025,7 +13031,7 @@
       <c r="IT42" s="10"/>
       <c r="IU42" s="11"/>
     </row>
-    <row r="43" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="12">
         <v>42</v>
       </c>
@@ -13290,7 +13296,7 @@
       <c r="IT43" s="10"/>
       <c r="IU43" s="11"/>
     </row>
-    <row r="44" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -13555,7 +13561,7 @@
       <c r="IT44" s="10"/>
       <c r="IU44" s="11"/>
     </row>
-    <row r="45" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="12">
         <v>44</v>
       </c>
@@ -13820,7 +13826,7 @@
       <c r="IT45" s="10"/>
       <c r="IU45" s="11"/>
     </row>
-    <row r="46" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="12">
         <v>45</v>
       </c>
@@ -14083,7 +14089,7 @@
       <c r="IT46" s="10"/>
       <c r="IU46" s="11"/>
     </row>
-    <row r="47" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
         <v>46</v>
       </c>
@@ -14348,7 +14354,7 @@
       <c r="IT47" s="10"/>
       <c r="IU47" s="11"/>
     </row>
-    <row r="48" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="12">
         <v>47</v>
       </c>
@@ -14611,7 +14617,7 @@
       <c r="IT48" s="10"/>
       <c r="IU48" s="11"/>
     </row>
-    <row r="49" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="12">
         <v>48</v>
       </c>
@@ -14876,7 +14882,7 @@
       <c r="IT49" s="10"/>
       <c r="IU49" s="11"/>
     </row>
-    <row r="50" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
         <v>49</v>
       </c>
@@ -15141,7 +15147,7 @@
       <c r="IT50" s="10"/>
       <c r="IU50" s="11"/>
     </row>
-    <row r="51" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="12">
         <v>50</v>
       </c>
@@ -15406,7 +15412,7 @@
       <c r="IT51" s="10"/>
       <c r="IU51" s="11"/>
     </row>
-    <row r="52" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="12">
         <v>51</v>
       </c>
@@ -15671,7 +15677,7 @@
       <c r="IT52" s="10"/>
       <c r="IU52" s="11"/>
     </row>
-    <row r="53" spans="1:255" ht="31.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:255" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
         <v>52</v>
       </c>
@@ -15936,7 +15942,7 @@
       <c r="IT53" s="10"/>
       <c r="IU53" s="11"/>
     </row>
-    <row r="54" spans="1:255" ht="31.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:255" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="12">
         <v>53</v>
       </c>
@@ -16201,7 +16207,7 @@
       <c r="IT54" s="10"/>
       <c r="IU54" s="11"/>
     </row>
-    <row r="55" spans="1:255" ht="31.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:255" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="12">
         <v>54</v>
       </c>
@@ -16466,7 +16472,7 @@
       <c r="IT55" s="10"/>
       <c r="IU55" s="11"/>
     </row>
-    <row r="56" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
         <v>55</v>
       </c>
@@ -16731,7 +16737,7 @@
       <c r="IT56" s="10"/>
       <c r="IU56" s="11"/>
     </row>
-    <row r="57" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="12">
         <v>56</v>
       </c>
@@ -16996,7 +17002,7 @@
       <c r="IT57" s="10"/>
       <c r="IU57" s="11"/>
     </row>
-    <row r="58" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="12">
         <v>57</v>
       </c>
@@ -17259,7 +17265,7 @@
       <c r="IT58" s="10"/>
       <c r="IU58" s="11"/>
     </row>
-    <row r="59" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
         <v>58</v>
       </c>
@@ -17522,7 +17528,7 @@
       <c r="IT59" s="10"/>
       <c r="IU59" s="11"/>
     </row>
-    <row r="60" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="12">
         <v>59</v>
       </c>
@@ -17787,7 +17793,7 @@
       <c r="IT60" s="10"/>
       <c r="IU60" s="11"/>
     </row>
-    <row r="61" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
@@ -18044,7 +18050,7 @@
       <c r="IT61" s="10"/>
       <c r="IU61" s="11"/>
     </row>
-    <row r="62" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -18301,7 +18307,7 @@
       <c r="IT62" s="10"/>
       <c r="IU62" s="11"/>
     </row>
-    <row r="63" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
@@ -18558,7 +18564,7 @@
       <c r="IT63" s="10"/>
       <c r="IU63" s="11"/>
     </row>
-    <row r="64" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -18815,7 +18821,7 @@
       <c r="IT64" s="10"/>
       <c r="IU64" s="11"/>
     </row>
-    <row r="65" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="14"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
@@ -19072,7 +19078,7 @@
       <c r="IT65" s="10"/>
       <c r="IU65" s="11"/>
     </row>
-    <row r="66" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="14"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
@@ -19329,7 +19335,7 @@
       <c r="IT66" s="10"/>
       <c r="IU66" s="11"/>
     </row>
-    <row r="67" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="8"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
@@ -19586,7 +19592,7 @@
       <c r="IT67" s="10"/>
       <c r="IU67" s="11"/>
     </row>
-    <row r="68" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="14"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -19843,7 +19849,7 @@
       <c r="IT68" s="10"/>
       <c r="IU68" s="11"/>
     </row>
-    <row r="69" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="8"/>
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
@@ -20100,7 +20106,7 @@
       <c r="IT69" s="10"/>
       <c r="IU69" s="11"/>
     </row>
-    <row r="70" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="14"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -20357,7 +20363,7 @@
       <c r="IT70" s="10"/>
       <c r="IU70" s="11"/>
     </row>
-    <row r="71" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="8"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
@@ -20614,7 +20620,7 @@
       <c r="IT71" s="10"/>
       <c r="IU71" s="11"/>
     </row>
-    <row r="72" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="15"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -20871,7 +20877,7 @@
       <c r="IT72" s="10"/>
       <c r="IU72" s="11"/>
     </row>
-    <row r="73" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="16"/>
       <c r="B73" s="14"/>
       <c r="C73" s="14"/>
@@ -21128,7 +21134,7 @@
       <c r="IT73" s="10"/>
       <c r="IU73" s="11"/>
     </row>
-    <row r="74" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="16"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -21385,7 +21391,7 @@
       <c r="IT74" s="10"/>
       <c r="IU74" s="11"/>
     </row>
-    <row r="75" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="16"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
@@ -21642,7 +21648,7 @@
       <c r="IT75" s="10"/>
       <c r="IU75" s="11"/>
     </row>
-    <row r="76" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="16"/>
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
@@ -21899,7 +21905,7 @@
       <c r="IT76" s="10"/>
       <c r="IU76" s="11"/>
     </row>
-    <row r="77" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="16"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
@@ -22156,7 +22162,7 @@
       <c r="IT77" s="10"/>
       <c r="IU77" s="11"/>
     </row>
-    <row r="78" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="16"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
@@ -22413,7 +22419,7 @@
       <c r="IT78" s="10"/>
       <c r="IU78" s="11"/>
     </row>
-    <row r="79" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="16"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
@@ -22670,7 +22676,7 @@
       <c r="IT79" s="10"/>
       <c r="IU79" s="11"/>
     </row>
-    <row r="80" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="16"/>
       <c r="B80" s="14"/>
       <c r="C80" s="14"/>
@@ -22927,7 +22933,7 @@
       <c r="IT80" s="10"/>
       <c r="IU80" s="11"/>
     </row>
-    <row r="81" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="17"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
@@ -23201,7 +23207,7 @@
       <selection activeCell="C16" sqref="C16:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.6640625" style="21" customWidth="1"/>
     <col min="2" max="2" width="45.83203125" style="21" customWidth="1"/>
@@ -23211,7 +23217,7 @@
     <col min="6" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -23228,7 +23234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -23245,7 +23251,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25">
         <v>2</v>
       </c>
@@ -23260,7 +23266,7 @@
       </c>
       <c r="E3" s="32"/>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="23">
         <v>3</v>
       </c>
@@ -23275,7 +23281,7 @@
       </c>
       <c r="E4" s="33"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25">
         <v>4</v>
       </c>
@@ -23290,7 +23296,7 @@
       </c>
       <c r="E5" s="32"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="23">
         <v>5</v>
       </c>
@@ -23305,7 +23311,7 @@
       </c>
       <c r="E6" s="33"/>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25">
         <v>6</v>
       </c>
@@ -23320,7 +23326,7 @@
       </c>
       <c r="E7" s="32"/>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="23">
         <v>7</v>
       </c>
@@ -23335,7 +23341,7 @@
       </c>
       <c r="E8" s="33"/>
     </row>
-    <row r="9" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25">
         <v>8</v>
       </c>
@@ -23350,7 +23356,7 @@
       </c>
       <c r="E9" s="32"/>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -23365,7 +23371,7 @@
       </c>
       <c r="E10" s="33"/>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -23380,7 +23386,7 @@
       </c>
       <c r="E11" s="26"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="23">
         <v>11</v>
       </c>
@@ -23395,7 +23401,7 @@
       </c>
       <c r="E12" s="27"/>
     </row>
-    <row r="13" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -23410,7 +23416,7 @@
       </c>
       <c r="E13" s="26"/>
     </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23">
         <v>13</v>
       </c>
@@ -23425,7 +23431,7 @@
       </c>
       <c r="E14" s="27"/>
     </row>
-    <row r="15" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="25">
         <v>14</v>
       </c>
@@ -23440,7 +23446,7 @@
       </c>
       <c r="E15" s="26"/>
     </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="23">
         <v>15</v>
       </c>
@@ -23455,7 +23461,7 @@
       </c>
       <c r="E16" s="27"/>
     </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="25">
         <v>16</v>
       </c>
@@ -23470,7 +23476,7 @@
       </c>
       <c r="E17" s="26"/>
     </row>
-    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="23">
         <v>17</v>
       </c>
@@ -23485,7 +23491,7 @@
       </c>
       <c r="E18" s="27"/>
     </row>
-    <row r="19" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="25">
         <v>18</v>
       </c>
@@ -23500,7 +23506,7 @@
       </c>
       <c r="E19" s="26"/>
     </row>
-    <row r="20" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="23">
         <v>19</v>
       </c>
@@ -23515,7 +23521,7 @@
       </c>
       <c r="E20" s="27"/>
     </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="25">
         <v>20</v>
       </c>
@@ -23530,56 +23536,56 @@
       </c>
       <c r="E21" s="26"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="27"/>
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="26"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="27"/>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="26"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="27"/>
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="26"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="27"/>
       <c r="B28" s="24"/>
       <c r="C28" s="27"/>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="26"/>
       <c r="B29" s="22"/>
       <c r="C29" s="26"/>
@@ -23603,10 +23609,10 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="28" customWidth="1"/>
     <col min="2" max="2" width="50" style="28" customWidth="1"/>
@@ -23616,7 +23622,7 @@
     <col min="6" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -23633,7 +23639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>108</v>
       </c>
@@ -23650,7 +23656,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>109</v>
       </c>
@@ -23667,7 +23673,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>110</v>
       </c>
@@ -23678,11 +23684,11 @@
         <v>35</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>111</v>
       </c>
@@ -23693,11 +23699,11 @@
         <v>35</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>112</v>
       </c>
@@ -23712,7 +23718,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>113</v>
       </c>
@@ -23727,7 +23733,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>114</v>
       </c>
@@ -23742,7 +23748,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>115</v>
       </c>
@@ -23757,7 +23763,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>116</v>
       </c>
@@ -23772,7 +23778,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>117</v>
       </c>
@@ -23787,7 +23793,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>118</v>
       </c>
@@ -23802,7 +23808,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>119</v>
       </c>
@@ -23817,7 +23823,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>120</v>
       </c>
@@ -23832,7 +23838,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>121</v>
       </c>
@@ -23847,7 +23853,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>122</v>
       </c>
@@ -23862,7 +23868,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>123</v>
       </c>
@@ -23877,7 +23883,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>124</v>
       </c>
@@ -23892,7 +23898,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>125</v>
       </c>
@@ -23907,7 +23913,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>126</v>
       </c>
@@ -23922,7 +23928,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>127</v>
       </c>
@@ -23937,7 +23943,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>128</v>
       </c>
@@ -23946,7 +23952,7 @@
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>129</v>
       </c>
@@ -23955,7 +23961,7 @@
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>130</v>
       </c>
@@ -23964,7 +23970,7 @@
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>89</v>
       </c>
@@ -23973,7 +23979,7 @@
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>131</v>
       </c>
@@ -23982,21 +23988,21 @@
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -24016,18 +24022,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="67" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -24044,7 +24050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -24059,7 +24065,7 @@
       </c>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -24074,7 +24080,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -24089,7 +24095,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -24104,7 +24110,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -24119,7 +24125,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -24134,7 +24140,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -24149,106 +24155,104 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>25</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>104</v>
+      </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>31</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
-        <v>10</v>
-      </c>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
-        <v>11</v>
-      </c>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
-        <v>12</v>
-      </c>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
-        <v>13</v>
-      </c>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
-        <v>14</v>
-      </c>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
-        <v>15</v>
-      </c>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
-        <v>16</v>
-      </c>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="F23" s="29"/>
     </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="F24" s="29"/>
     </row>
-    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="F25" s="29"/>
     </row>
-    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="F26" s="29"/>
     </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="F27" s="29"/>
     </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="F28" s="29"/>
     </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="F29" s="30"/>
     </row>
   </sheetData>
@@ -24260,18 +24264,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="67" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -24288,7 +24292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -24303,7 +24307,7 @@
       </c>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -24318,7 +24322,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -24333,7 +24337,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -24348,7 +24352,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -24357,7 +24361,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -24366,7 +24370,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -24375,7 +24379,7 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -24384,7 +24388,7 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -24393,7 +24397,7 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -24402,7 +24406,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -24411,7 +24415,7 @@
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -24420,7 +24424,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -24429,7 +24433,7 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -24438,7 +24442,7 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -24447,7 +24451,7 @@
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="7">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Updated Product backlog for Nov13-Nov20.
</commit_message>
<xml_diff>
--- a/SSW695/product backlog.xlsx
+++ b/SSW695/product backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040"/>
   </bookViews>
   <sheets>
     <sheet name="product backlog" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="137">
   <si>
     <t>User Story</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>Pranay, Sonali</t>
-  </si>
-  <si>
-    <t>Create Api for post issue and get issue feed/history</t>
   </si>
   <si>
     <t>Create Api for forgot and reset password</t>
@@ -442,6 +439,9 @@
   </si>
   <si>
     <t>Create Api to update issue</t>
+  </si>
+  <si>
+    <t>Create Api for get issue feed/history</t>
   </si>
 </sst>
 </file>
@@ -1895,10 +1895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IU81"/>
+  <dimension ref="A1:IU82"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:C32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -8540,15 +8540,17 @@
     </row>
     <row r="26" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
-        <v>25</v>
+        <v>25.1</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="8"/>
+      <c r="D26" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="9"/>
       <c r="G26" s="10"/>
@@ -8802,17 +8804,19 @@
       <c r="IU26" s="11"/>
     </row>
     <row r="27" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="12">
-        <v>26</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="13" t="s">
+      <c r="A27" s="6">
+        <v>25.2</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+      <c r="D27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="8"/>
       <c r="F27" s="9"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
@@ -9065,17 +9069,19 @@
       <c r="IU27" s="11"/>
     </row>
     <row r="28" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
-        <v>27</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="7" t="s">
+      <c r="A28" s="12">
+        <v>26</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="D28" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="14"/>
       <c r="F28" s="9"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -9328,19 +9334,17 @@
       <c r="IU28" s="11"/>
     </row>
     <row r="29" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="12">
-        <v>28</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="13" t="s">
+      <c r="A29" s="6">
+        <v>27</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="13" t="s">
-        <v>40</v>
-      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
       <c r="F29" s="9"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -9593,17 +9597,19 @@
       <c r="IU29" s="11"/>
     </row>
     <row r="30" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="6">
-        <v>29</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="7" t="s">
+      <c r="A30" s="12">
+        <v>28</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="F30" s="9"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
@@ -9856,17 +9862,17 @@
       <c r="IU30" s="11"/>
     </row>
     <row r="31" spans="1:255" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="12">
-        <v>30</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="13" t="s">
+      <c r="A31" s="6">
+        <v>29</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
       <c r="F31" s="9"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
@@ -10119,19 +10125,17 @@
       <c r="IU31" s="11"/>
     </row>
     <row r="32" spans="1:255" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="6">
-        <v>31</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="7" t="s">
+      <c r="A32" s="12">
+        <v>30</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="7" t="s">
-        <v>44</v>
-      </c>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
       <c r="F32" s="9"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
@@ -10384,18 +10388,18 @@
       <c r="IU32" s="11"/>
     </row>
     <row r="33" spans="1:255" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="12">
-        <v>32</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="13" t="s">
+      <c r="A33" s="6">
+        <v>31</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="13" t="s">
-        <v>46</v>
+      <c r="D33" s="8"/>
+      <c r="E33" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="10"/>
@@ -10650,16 +10654,18 @@
     </row>
     <row r="34" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
-        <v>33</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="F34" s="9"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -10912,17 +10918,19 @@
       <c r="IU34" s="11"/>
     </row>
     <row r="35" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="6">
-        <v>34</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="13" t="s">
+      <c r="A35" s="12">
+        <v>33</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="14"/>
+      <c r="D35" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="8"/>
       <c r="F35" s="9"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
@@ -11175,17 +11183,19 @@
       <c r="IU35" s="11"/>
     </row>
     <row r="36" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12">
+      <c r="A36" s="6">
+        <v>34</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
+      <c r="D36" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="14"/>
       <c r="F36" s="9"/>
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
@@ -11439,20 +11449,18 @@
     </row>
     <row r="37" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12">
-        <v>36</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>51</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="7"/>
       <c r="F37" s="9"/>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
@@ -11705,20 +11713,20 @@
       <c r="IU37" s="11"/>
     </row>
     <row r="38" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="6">
-        <v>37</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="7" t="s">
+      <c r="A38" s="12">
+        <v>36</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>53</v>
+      <c r="E38" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="10"/>
@@ -11972,19 +11980,21 @@
       <c r="IU38" s="11"/>
     </row>
     <row r="39" spans="1:255" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="12">
-        <v>38</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" s="14"/>
+      <c r="A39" s="6">
+        <v>37</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="F39" s="9"/>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
@@ -12238,18 +12248,18 @@
     </row>
     <row r="40" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="12">
-        <v>39</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="8"/>
+        <v>38</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="14"/>
       <c r="F40" s="9"/>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
@@ -12502,19 +12512,19 @@
       <c r="IU40" s="11"/>
     </row>
     <row r="41" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="6">
-        <v>40</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="13" t="s">
+      <c r="A41" s="12">
+        <v>39</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="C41" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="14"/>
+      <c r="E41" s="8"/>
       <c r="F41" s="9"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
@@ -12767,19 +12777,19 @@
       <c r="IU41" s="11"/>
     </row>
     <row r="42" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="12">
-        <v>41</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D42" s="7" t="s">
+      <c r="A42" s="6">
+        <v>40</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="8"/>
+      <c r="E42" s="14"/>
       <c r="F42" s="9"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
@@ -13033,18 +13043,18 @@
     </row>
     <row r="43" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="12">
-        <v>42</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D43" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="14"/>
+      <c r="E43" s="8"/>
       <c r="F43" s="9"/>
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
@@ -13297,19 +13307,19 @@
       <c r="IU43" s="11"/>
     </row>
     <row r="44" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="6">
-        <v>43</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E44" s="8"/>
+      <c r="A44" s="12">
+        <v>42</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="14"/>
       <c r="F44" s="9"/>
       <c r="G44" s="10"/>
       <c r="H44" s="10"/>
@@ -13562,19 +13572,19 @@
       <c r="IU44" s="11"/>
     </row>
     <row r="45" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="12">
-        <v>44</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D45" s="13" t="s">
+      <c r="A45" s="6">
+        <v>43</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="14"/>
+      <c r="E45" s="8"/>
       <c r="F45" s="9"/>
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
@@ -13828,16 +13838,18 @@
     </row>
     <row r="46" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="12">
-        <v>45</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
+        <v>44</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="14"/>
       <c r="F46" s="9"/>
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
@@ -14090,19 +14102,17 @@
       <c r="IU46" s="11"/>
     </row>
     <row r="47" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="6">
-        <v>46</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="14"/>
+      <c r="A47" s="12">
+        <v>45</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
       <c r="F47" s="9"/>
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
@@ -14355,17 +14365,19 @@
       <c r="IU47" s="11"/>
     </row>
     <row r="48" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="12">
-        <v>47</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
+      <c r="A48" s="6">
+        <v>46</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="14"/>
       <c r="F48" s="9"/>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
@@ -14619,18 +14631,16 @@
     </row>
     <row r="49" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="12">
-        <v>48</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
       <c r="F49" s="9"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
@@ -14883,19 +14893,19 @@
       <c r="IU49" s="11"/>
     </row>
     <row r="50" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="6">
-        <v>49</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" s="8"/>
+      <c r="A50" s="12">
+        <v>48</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="14"/>
       <c r="F50" s="9"/>
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
@@ -15148,19 +15158,19 @@
       <c r="IU50" s="11"/>
     </row>
     <row r="51" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="12">
-        <v>50</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D51" s="13" t="s">
+      <c r="A51" s="6">
+        <v>49</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E51" s="14"/>
+      <c r="E51" s="8"/>
       <c r="F51" s="9"/>
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
@@ -15414,18 +15424,18 @@
     </row>
     <row r="52" spans="1:255" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="12">
-        <v>51</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D52" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E52" s="8"/>
+      <c r="E52" s="14"/>
       <c r="F52" s="9"/>
       <c r="G52" s="10"/>
       <c r="H52" s="10"/>
@@ -15678,19 +15688,19 @@
       <c r="IU52" s="11"/>
     </row>
     <row r="53" spans="1:255" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="6">
-        <v>52</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C53" s="13" t="s">
+      <c r="A53" s="12">
+        <v>51</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D53" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E53" s="14"/>
+      <c r="E53" s="8"/>
       <c r="F53" s="9"/>
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
@@ -15943,19 +15953,19 @@
       <c r="IU53" s="11"/>
     </row>
     <row r="54" spans="1:255" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="12">
-        <v>53</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C54" s="7" t="s">
+      <c r="A54" s="6">
+        <v>52</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E54" s="8"/>
+      <c r="E54" s="14"/>
       <c r="F54" s="9"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
@@ -16209,18 +16219,18 @@
     </row>
     <row r="55" spans="1:255" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="12">
-        <v>54</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E55" s="14"/>
+        <v>53</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" s="8"/>
       <c r="F55" s="9"/>
       <c r="G55" s="10"/>
       <c r="H55" s="10"/>
@@ -16473,19 +16483,19 @@
       <c r="IU55" s="11"/>
     </row>
     <row r="56" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="6">
-        <v>55</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C56" s="7" t="s">
+      <c r="A56" s="12">
+        <v>54</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E56" s="8"/>
+      <c r="D56" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="14"/>
       <c r="F56" s="9"/>
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
@@ -16738,19 +16748,19 @@
       <c r="IU56" s="11"/>
     </row>
     <row r="57" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="12">
-        <v>56</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C57" s="13" t="s">
+      <c r="A57" s="6">
+        <v>55</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D57" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E57" s="14"/>
+      <c r="E57" s="8"/>
       <c r="F57" s="9"/>
       <c r="G57" s="10"/>
       <c r="H57" s="10"/>
@@ -17004,16 +17014,18 @@
     </row>
     <row r="58" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="12">
-        <v>57</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
+        <v>56</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="14"/>
       <c r="F58" s="9"/>
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
@@ -17266,17 +17278,17 @@
       <c r="IU58" s="11"/>
     </row>
     <row r="59" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="6">
-        <v>58</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
+      <c r="A59" s="12">
+        <v>57</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
       <c r="F59" s="9"/>
       <c r="G59" s="10"/>
       <c r="H59" s="10"/>
@@ -17529,19 +17541,17 @@
       <c r="IU59" s="11"/>
     </row>
     <row r="60" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="12">
-        <v>59</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E60" s="8"/>
+      <c r="A60" s="6">
+        <v>58</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
       <c r="F60" s="9"/>
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>
@@ -17794,10 +17804,18 @@
       <c r="IU60" s="11"/>
     </row>
     <row r="61" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="14"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
+      <c r="A61" s="12">
+        <v>59</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E61" s="8"/>
       <c r="F61" s="9"/>
       <c r="G61" s="10"/>
@@ -18051,11 +18069,11 @@
       <c r="IU61" s="11"/>
     </row>
     <row r="62" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="8"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="14"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="8"/>
       <c r="F62" s="9"/>
       <c r="G62" s="10"/>
       <c r="H62" s="10"/>
@@ -18308,11 +18326,11 @@
       <c r="IU62" s="11"/>
     </row>
     <row r="63" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="8"/>
+      <c r="A63" s="8"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="14"/>
       <c r="F63" s="9"/>
       <c r="G63" s="10"/>
       <c r="H63" s="10"/>
@@ -18565,11 +18583,11 @@
       <c r="IU63" s="11"/>
     </row>
     <row r="64" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="14"/>
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="8"/>
       <c r="F64" s="9"/>
       <c r="G64" s="10"/>
       <c r="H64" s="10"/>
@@ -18822,11 +18840,11 @@
       <c r="IU64" s="11"/>
     </row>
     <row r="65" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="14"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="8"/>
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="14"/>
       <c r="F65" s="9"/>
       <c r="G65" s="10"/>
       <c r="H65" s="10"/>
@@ -19080,10 +19098,10 @@
     </row>
     <row r="66" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="14"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="8"/>
       <c r="F66" s="9"/>
       <c r="G66" s="10"/>
       <c r="H66" s="10"/>
@@ -19336,11 +19354,11 @@
       <c r="IU66" s="11"/>
     </row>
     <row r="67" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="8"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="8"/>
+      <c r="A67" s="14"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="14"/>
       <c r="F67" s="9"/>
       <c r="G67" s="10"/>
       <c r="H67" s="10"/>
@@ -19593,11 +19611,11 @@
       <c r="IU67" s="11"/>
     </row>
     <row r="68" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="14"/>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="14"/>
+      <c r="A68" s="8"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="8"/>
       <c r="F68" s="9"/>
       <c r="G68" s="10"/>
       <c r="H68" s="10"/>
@@ -19850,11 +19868,11 @@
       <c r="IU68" s="11"/>
     </row>
     <row r="69" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="8"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="8"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="14"/>
       <c r="F69" s="9"/>
       <c r="G69" s="10"/>
       <c r="H69" s="10"/>
@@ -20107,11 +20125,11 @@
       <c r="IU69" s="11"/>
     </row>
     <row r="70" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="14"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="14"/>
+      <c r="A70" s="8"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="8"/>
       <c r="F70" s="9"/>
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>
@@ -20364,11 +20382,11 @@
       <c r="IU70" s="11"/>
     </row>
     <row r="71" spans="1:255" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="8"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="8"/>
+      <c r="A71" s="14"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="14"/>
       <c r="F71" s="9"/>
       <c r="G71" s="10"/>
       <c r="H71" s="10"/>
@@ -20621,11 +20639,11 @@
       <c r="IU71" s="11"/>
     </row>
     <row r="72" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="15"/>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="14"/>
+      <c r="A72" s="8"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="8"/>
       <c r="F72" s="9"/>
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
@@ -20878,11 +20896,11 @@
       <c r="IU72" s="11"/>
     </row>
     <row r="73" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="16"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="8"/>
+      <c r="A73" s="15"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="14"/>
       <c r="F73" s="9"/>
       <c r="G73" s="10"/>
       <c r="H73" s="10"/>
@@ -21136,10 +21154,10 @@
     </row>
     <row r="74" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="16"/>
-      <c r="B74" s="8"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="8"/>
       <c r="F74" s="9"/>
       <c r="G74" s="10"/>
       <c r="H74" s="10"/>
@@ -21393,10 +21411,10 @@
     </row>
     <row r="75" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="16"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="8"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="14"/>
       <c r="F75" s="9"/>
       <c r="G75" s="10"/>
       <c r="H75" s="10"/>
@@ -21653,7 +21671,7 @@
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
       <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
+      <c r="E76" s="8"/>
       <c r="F76" s="9"/>
       <c r="G76" s="10"/>
       <c r="H76" s="10"/>
@@ -21907,10 +21925,10 @@
     </row>
     <row r="77" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="16"/>
-      <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
       <c r="F77" s="9"/>
       <c r="G77" s="10"/>
       <c r="H77" s="10"/>
@@ -22164,10 +22182,10 @@
     </row>
     <row r="78" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="16"/>
-      <c r="B78" s="14"/>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
       <c r="F78" s="9"/>
       <c r="G78" s="10"/>
       <c r="H78" s="10"/>
@@ -22421,10 +22439,10 @@
     </row>
     <row r="79" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="16"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
       <c r="F79" s="9"/>
       <c r="G79" s="10"/>
       <c r="H79" s="10"/>
@@ -22678,10 +22696,10 @@
     </row>
     <row r="80" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="16"/>
-      <c r="B80" s="14"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
       <c r="F80" s="9"/>
       <c r="G80" s="10"/>
       <c r="H80" s="10"/>
@@ -22934,11 +22952,11 @@
       <c r="IU80" s="11"/>
     </row>
     <row r="81" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="17"/>
-      <c r="B81" s="8"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
+      <c r="A81" s="16"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
       <c r="F81" s="18"/>
       <c r="G81" s="19"/>
       <c r="H81" s="19"/>
@@ -23190,6 +23208,13 @@
       <c r="IT81" s="19"/>
       <c r="IU81" s="20"/>
     </row>
+    <row r="82" spans="1:255" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="17"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -23239,7 +23264,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>6</v>
@@ -23248,7 +23273,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -23256,7 +23281,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>6</v>
@@ -23271,7 +23296,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>6</v>
@@ -23286,7 +23311,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>6</v>
@@ -23301,7 +23326,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>6</v>
@@ -23316,7 +23341,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>6</v>
@@ -23331,7 +23356,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>6</v>
@@ -23346,7 +23371,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>6</v>
@@ -23361,7 +23386,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>6</v>
@@ -23451,10 +23476,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="24" t="s">
         <v>87</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>88</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>7</v>
@@ -23466,7 +23491,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>32</v>
@@ -23481,7 +23506,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="24" t="s">
         <v>32</v>
@@ -23496,7 +23521,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>32</v>
@@ -23511,7 +23536,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="24" t="s">
         <v>32</v>
@@ -23526,7 +23551,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>32</v>
@@ -23641,10 +23666,10 @@
     </row>
     <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>35</v>
@@ -23653,15 +23678,15 @@
         <v>7</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>35</v>
@@ -23670,15 +23695,15 @@
         <v>17</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>35</v>
@@ -23690,10 +23715,10 @@
     </row>
     <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>35</v>
@@ -23705,10 +23730,10 @@
     </row>
     <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>32</v>
@@ -23720,10 +23745,10 @@
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>32</v>
@@ -23735,10 +23760,10 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>32</v>
@@ -23750,10 +23775,10 @@
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>28</v>
@@ -23765,10 +23790,10 @@
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>28</v>
@@ -23780,10 +23805,10 @@
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>28</v>
@@ -23795,10 +23820,10 @@
     </row>
     <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>6</v>
@@ -23810,10 +23835,10 @@
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>6</v>
@@ -23825,10 +23850,10 @@
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>6</v>
@@ -23840,10 +23865,10 @@
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>6</v>
@@ -23855,10 +23880,10 @@
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>6</v>
@@ -23870,10 +23895,10 @@
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>6</v>
@@ -23885,10 +23910,10 @@
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>6</v>
@@ -23900,13 +23925,13 @@
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>17</v>
@@ -23915,10 +23940,10 @@
     </row>
     <row r="20" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>30</v>
@@ -23930,10 +23955,10 @@
     </row>
     <row r="21" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>30</v>
@@ -23945,7 +23970,7 @@
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -23954,7 +23979,7 @@
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -23963,7 +23988,7 @@
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -23972,7 +23997,7 @@
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -23981,7 +24006,7 @@
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -24022,8 +24047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -24055,7 +24080,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>32</v>
@@ -24070,7 +24095,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>32</v>
@@ -24085,7 +24110,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>32</v>
@@ -24100,7 +24125,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>32</v>
@@ -24115,7 +24140,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>32</v>
@@ -24130,13 +24155,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" s="7"/>
     </row>
@@ -24145,7 +24170,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>28</v>
@@ -24157,16 +24182,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
-        <v>25</v>
+        <v>25.1</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E9" s="7"/>
     </row>
@@ -24175,13 +24200,13 @@
         <v>31</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E10" s="7"/>
     </row>
@@ -24265,7 +24290,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -24297,7 +24322,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>32</v>
@@ -24312,7 +24337,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>32</v>
@@ -24327,7 +24352,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>28</v>
@@ -24342,7 +24367,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>28</v>
@@ -24353,108 +24378,100 @@
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="A6" s="6">
+        <v>25.2</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="A7" s="12">
+        <v>35</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="7">
-        <v>7</v>
-      </c>
+      <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
+      <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="7">
-        <v>9</v>
-      </c>
+      <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="7">
-        <v>10</v>
-      </c>
+      <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="7">
-        <v>11</v>
-      </c>
+      <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="7">
-        <v>12</v>
-      </c>
+      <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="7">
-        <v>13</v>
-      </c>
+      <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="7">
-        <v>14</v>
-      </c>
+      <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="7">
-        <v>15</v>
-      </c>
+      <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="7">
-        <v>16</v>
-      </c>
+      <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>

</xml_diff>